<commit_message>
Added ftest for windows
</commit_message>
<xml_diff>
--- a/ftest/ftest.xlsx
+++ b/ftest/ftest.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\Joh\git\ktest\ftest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\Joh\testgit\ktest\ftest\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="83">
   <si>
     <t>yes</t>
   </si>
@@ -211,13 +211,76 @@
   </si>
   <si>
     <t>Functionality:</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>complete (installer test)</t>
+  </si>
+  <si>
+    <t>results checked</t>
+  </si>
+  <si>
+    <t>broken</t>
+  </si>
+  <si>
+    <t>fm3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WE1 Residential policy with multiple coverages and separate coverage terms. </t>
+  </si>
+  <si>
+    <t>Windows</t>
+  </si>
+  <si>
+    <t>Linux</t>
+  </si>
+  <si>
+    <t>not done</t>
+  </si>
+  <si>
+    <t>WE2 Residential policy with multiple coverages and combined property coverage terms.</t>
+  </si>
+  <si>
+    <t>fm4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WE3 Residential policy with multiple coverages and combined location coverage terms. </t>
+  </si>
+  <si>
+    <t>fm5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WE4 Residential policy with multiple coverages and locations and blanket policy terms. </t>
+  </si>
+  <si>
+    <t>fm6</t>
+  </si>
+  <si>
+    <t>WE5 Residential policy with coverage deductibles and blanket policy terms.</t>
+  </si>
+  <si>
+    <t>fm7</t>
+  </si>
+  <si>
+    <t>-1,0</t>
+  </si>
+  <si>
+    <t>12,1</t>
+  </si>
+  <si>
+    <t>3,1</t>
+  </si>
+  <si>
+    <t>Notes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -235,6 +298,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -275,14 +345,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -563,118 +645,297 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H7"/>
+  <dimension ref="B1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="48.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="69.42578125" customWidth="1"/>
+    <col min="9" max="9" width="22.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="4" t="s">
+      <c r="I3" t="s">
+        <v>68</v>
+      </c>
+      <c r="J3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="3" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="I4" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I5" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>4</v>
       </c>
       <c r="C6" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="5" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I6" t="s">
+        <v>64</v>
+      </c>
+      <c r="J6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>13</v>
       </c>
       <c r="C7" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="5" t="s">
         <v>57</v>
+      </c>
+      <c r="I7" t="s">
+        <v>65</v>
+      </c>
+      <c r="J7" t="s">
+        <v>70</v>
+      </c>
+      <c r="K7" s="5"/>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" s="5">
+        <v>0</v>
+      </c>
+      <c r="E8" s="5">
+        <v>1</v>
+      </c>
+      <c r="F8" s="5">
+        <v>1</v>
+      </c>
+      <c r="G8" s="5">
+        <v>1</v>
+      </c>
+      <c r="H8" s="5">
+        <v>1</v>
+      </c>
+      <c r="I8" t="s">
+        <v>64</v>
+      </c>
+      <c r="J8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9" t="s">
+        <v>64</v>
+      </c>
+      <c r="J9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" t="s">
+        <v>73</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10" t="s">
+        <v>64</v>
+      </c>
+      <c r="J10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11" t="s">
+        <v>75</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11" s="5">
+        <v>1</v>
+      </c>
+      <c r="F11" s="5">
+        <v>1</v>
+      </c>
+      <c r="G11" s="5">
+        <v>1</v>
+      </c>
+      <c r="H11" s="5">
+        <v>1</v>
+      </c>
+      <c r="I11" t="s">
+        <v>64</v>
+      </c>
+      <c r="J11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G12" s="5">
+        <v>1</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="I12" t="s">
+        <v>64</v>
+      </c>
+      <c r="J12" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -687,7 +948,7 @@
   <dimension ref="B2:I24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -700,395 +961,395 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="3" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="3">
-        <v>1</v>
-      </c>
-      <c r="E4" s="3">
-        <v>1</v>
-      </c>
-      <c r="F4" s="3">
-        <v>1</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I4" s="3" t="s">
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <v>2</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>3</v>
       </c>
-      <c r="F5" s="3">
-        <v>1</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="I5" s="3" t="s">
+      <c r="F5" s="2">
+        <v>1</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I5" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="2">
         <v>3</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="2">
         <v>12</v>
       </c>
-      <c r="F6" s="3">
-        <v>1</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I6" s="3" t="s">
+      <c r="F6" s="2">
+        <v>1</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I6" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="2">
         <v>4</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="2">
         <v>10</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="2">
         <v>3</v>
       </c>
-      <c r="H7" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="I7" s="3" t="s">
+      <c r="H7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="2">
         <v>5</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="2">
         <v>11</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="2">
         <v>3</v>
       </c>
-      <c r="H8" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="I8" s="3" t="s">
+      <c r="H8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I8" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="2">
         <v>6</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="2">
         <v>2</v>
       </c>
-      <c r="F9" s="3">
-        <v>1</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I9" s="3" t="s">
+      <c r="F9" s="2">
+        <v>1</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I9" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="2">
         <v>7</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="2">
         <v>13</v>
       </c>
-      <c r="F10" s="3">
-        <v>1</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="I10" s="3" t="s">
+      <c r="F10" s="2">
+        <v>1</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I10" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="2">
         <v>8</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="2">
         <v>6</v>
       </c>
-      <c r="F11" s="3">
-        <v>1</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="I11" s="3" t="s">
+      <c r="F11" s="2">
+        <v>1</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I11" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="2">
         <v>9</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="2">
         <v>4</v>
       </c>
-      <c r="F12" s="3">
-        <v>1</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="I12" s="3" t="s">
+      <c r="F12" s="2">
+        <v>1</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I12" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="2">
         <v>10</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="2">
         <v>5</v>
       </c>
-      <c r="F13" s="3">
-        <v>1</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="I13" s="3" t="s">
+      <c r="F13" s="2">
+        <v>1</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I13" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="2">
         <v>11</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="2">
         <v>9</v>
       </c>
-      <c r="F14" s="3">
-        <v>1</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="I14" s="3" t="s">
+      <c r="F14" s="2">
+        <v>1</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I14" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="2">
         <v>12</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="2">
         <v>14</v>
       </c>
-      <c r="F15" s="3">
-        <v>1</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="I15" s="3" t="s">
+      <c r="F15" s="2">
+        <v>1</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I15" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H18" s="4" t="s">
+      <c r="H18" s="3" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H19" s="2" t="s">
+      <c r="H19" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="I19" s="2" t="s">
+      <c r="I19" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="2">
         <v>-1</v>
       </c>
-      <c r="H20" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I20" s="3" t="s">
+      <c r="H20" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I20" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C21" s="3">
-        <v>0</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I21" s="3" t="s">
+      <c r="C21" s="2">
+        <v>0</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I21" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C22" s="3">
-        <v>1</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I22" s="3" t="s">
+      <c r="C22" s="2">
+        <v>1</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I22" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23" s="2">
         <v>2</v>
       </c>
-      <c r="H23" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="I23" s="3" t="s">
+      <c r="H23" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I23" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C24" s="3">
+      <c r="C24" s="2">
         <v>3</v>
       </c>
-      <c r="H24" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="I24" s="3" t="s">
+      <c r="H24" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I24" s="2" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added ftests for min and max deductibles
</commit_message>
<xml_diff>
--- a/ftest/ftest.xlsx
+++ b/ftest/ftest.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="89">
   <si>
     <t>yes</t>
   </si>
@@ -219,12 +219,6 @@
     <t>complete (installer test)</t>
   </si>
   <si>
-    <t>results checked</t>
-  </si>
-  <si>
-    <t>broken</t>
-  </si>
-  <si>
     <t>fm3</t>
   </si>
   <si>
@@ -274,6 +268,30 @@
   </si>
   <si>
     <t>Notes</t>
+  </si>
+  <si>
+    <t>fm8</t>
+  </si>
+  <si>
+    <t>complete</t>
+  </si>
+  <si>
+    <t>invalid (to replace)</t>
+  </si>
+  <si>
+    <t>Maximum deductible</t>
+  </si>
+  <si>
+    <t>fm9</t>
+  </si>
+  <si>
+    <t>Minimum deductible</t>
+  </si>
+  <si>
+    <t>3,4,12</t>
+  </si>
+  <si>
+    <t>new fmcalc only</t>
   </si>
 </sst>
 </file>
@@ -345,24 +363,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -645,16 +658,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:K12"/>
+  <dimension ref="B1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="69.42578125" customWidth="1"/>
     <col min="9" max="9" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" x14ac:dyDescent="0.25">
@@ -667,10 +681,10 @@
         <v>61</v>
       </c>
       <c r="I3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
@@ -702,240 +716,311 @@
         <v>62</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="I5" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="J5" s="5" t="s">
         <v>63</v>
       </c>
+      <c r="K5" s="5"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="B6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="K6" s="5"/>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="K7" s="7"/>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B8" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="J6" t="s">
+      <c r="C8" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" s="7">
+        <v>0</v>
+      </c>
+      <c r="E8" s="7">
+        <v>1</v>
+      </c>
+      <c r="F8" s="7">
+        <v>1</v>
+      </c>
+      <c r="G8" s="7">
+        <v>1</v>
+      </c>
+      <c r="H8" s="7">
+        <v>1</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="K8" s="5"/>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B9" s="5" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" s="5" t="s">
+      <c r="C9" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D9" s="5">
+        <v>0</v>
+      </c>
+      <c r="E9" s="5">
+        <v>1</v>
+      </c>
+      <c r="F9" s="5">
+        <v>1</v>
+      </c>
+      <c r="G9" s="5">
+        <v>1</v>
+      </c>
+      <c r="H9" s="5">
+        <v>1</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="K9" s="5"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B10" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D10" s="5">
+        <v>0</v>
+      </c>
+      <c r="E10" s="5">
+        <v>1</v>
+      </c>
+      <c r="F10" s="5">
+        <v>1</v>
+      </c>
+      <c r="G10" s="5">
+        <v>1</v>
+      </c>
+      <c r="H10" s="5">
+        <v>1</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="K10" s="5"/>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B11" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D11" s="5">
+        <v>0</v>
+      </c>
+      <c r="E11" s="7">
+        <v>1</v>
+      </c>
+      <c r="F11" s="7">
+        <v>1</v>
+      </c>
+      <c r="G11" s="7">
+        <v>1</v>
+      </c>
+      <c r="H11" s="7">
+        <v>1</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="K11" s="5"/>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="G12" s="7">
+        <v>1</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="K12" s="5"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D13" s="5">
+        <v>0</v>
+      </c>
+      <c r="E13" s="7">
+        <v>10</v>
+      </c>
+      <c r="F13" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="G7" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="I7" t="s">
-        <v>65</v>
-      </c>
-      <c r="J7" t="s">
-        <v>70</v>
-      </c>
-      <c r="K7" s="5"/>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>66</v>
-      </c>
-      <c r="C8" t="s">
-        <v>67</v>
-      </c>
-      <c r="D8" s="5">
-        <v>0</v>
-      </c>
-      <c r="E8" s="5">
-        <v>1</v>
-      </c>
-      <c r="F8" s="5">
-        <v>1</v>
-      </c>
-      <c r="G8" s="5">
-        <v>1</v>
-      </c>
-      <c r="H8" s="5">
-        <v>1</v>
-      </c>
-      <c r="I8" t="s">
-        <v>64</v>
-      </c>
-      <c r="J8" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>72</v>
-      </c>
-      <c r="C9" t="s">
-        <v>71</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
-      <c r="H9">
-        <v>1</v>
-      </c>
-      <c r="I9" t="s">
-        <v>64</v>
-      </c>
-      <c r="J9" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>74</v>
-      </c>
-      <c r="C10" t="s">
-        <v>73</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-      <c r="H10">
-        <v>1</v>
-      </c>
-      <c r="I10" t="s">
-        <v>64</v>
-      </c>
-      <c r="J10" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>76</v>
-      </c>
-      <c r="C11" t="s">
-        <v>75</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11" s="5">
-        <v>1</v>
-      </c>
-      <c r="F11" s="5">
-        <v>1</v>
-      </c>
-      <c r="G11" s="5">
-        <v>1</v>
-      </c>
-      <c r="H11" s="5">
-        <v>1</v>
-      </c>
-      <c r="I11" t="s">
-        <v>64</v>
-      </c>
-      <c r="J11" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>78</v>
-      </c>
-      <c r="C12" t="s">
-        <v>77</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="G12" s="5">
-        <v>1</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="I12" t="s">
-        <v>64</v>
-      </c>
-      <c r="J12" t="s">
-        <v>70</v>
+      <c r="G13" s="7">
+        <v>1</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="K13" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D14" s="5">
+        <v>0</v>
+      </c>
+      <c r="E14" s="7">
+        <v>11</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="G14" s="7">
+        <v>1</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="K14" s="7" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -948,7 +1033,7 @@
   <dimension ref="B2:I24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1238,7 +1323,7 @@
         <v>1</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
@@ -1261,7 +1346,7 @@
         <v>1</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
@@ -1322,7 +1407,7 @@
         <v>0</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
@@ -1350,7 +1435,7 @@
         <v>1</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added fm10 test franchise deductible
</commit_message>
<xml_diff>
--- a/ftest/ftest.xlsx
+++ b/ftest/ftest.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="94">
   <si>
     <t>yes</t>
   </si>
@@ -292,6 +292,21 @@
   </si>
   <si>
     <t>new fmcalc only</t>
+  </si>
+  <si>
+    <t>fm10</t>
+  </si>
+  <si>
+    <t>Franchise deductible</t>
+  </si>
+  <si>
+    <t>fm11</t>
+  </si>
+  <si>
+    <t>Deductible and limit as a proportion of loss</t>
+  </si>
+  <si>
+    <t>to do</t>
   </si>
 </sst>
 </file>
@@ -658,10 +673,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:K14"/>
+  <dimension ref="B1:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1022,6 +1037,74 @@
       <c r="K14" s="7" t="s">
         <v>88</v>
       </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D15" s="5">
+        <v>0</v>
+      </c>
+      <c r="E15" s="7">
+        <v>3</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15" s="7">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>2</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="K15" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D16" s="5">
+        <v>0</v>
+      </c>
+      <c r="E16" s="7">
+        <v>5</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16" s="7">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>10</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="K16" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added tests 11, 13, 14, 15
</commit_message>
<xml_diff>
--- a/ftest/ftest.xlsx
+++ b/ftest/ftest.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\Joh\git\ktest\ftest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\Joh\testgit\ktest\ftest\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="90">
   <si>
     <t>yes</t>
   </si>
@@ -81,9 +81,6 @@
     <t>ProfileDescription</t>
   </si>
   <si>
-    <t>ProfileName</t>
-  </si>
-  <si>
     <t>ProfileID</t>
   </si>
   <si>
@@ -96,75 +93,39 @@
     <t>Deductible and Limit (Function1)</t>
   </si>
   <si>
-    <t>A_1</t>
-  </si>
-  <si>
     <t>Franchise Deductible and Limit (Function 3)</t>
   </si>
   <si>
-    <t>A_2</t>
-  </si>
-  <si>
     <t>Deductible only (Function 12)</t>
   </si>
   <si>
-    <t>B_1</t>
-  </si>
-  <si>
     <t>Deductible as a cap on the retention of input losses (Function 10)</t>
   </si>
   <si>
-    <t>B_2</t>
-  </si>
-  <si>
     <t>Deductible as a floor on the retention of input losses (Function 11)</t>
   </si>
   <si>
-    <t>B_3</t>
-  </si>
-  <si>
     <t>Deductible, Limit and Share (Function2)</t>
   </si>
   <si>
-    <t>C_1</t>
-  </si>
-  <si>
     <t>Excess, Coverage and Share (Function13)</t>
   </si>
   <si>
-    <t>C_2</t>
-  </si>
-  <si>
     <t>Deductible as a proportion of TIV (Function 6)</t>
   </si>
   <si>
-    <t>D_1</t>
-  </si>
-  <si>
     <t>Deductible and Limit as a proportion of TIV (Function 4)</t>
   </si>
   <si>
-    <t>E_1</t>
-  </si>
-  <si>
     <t>Deductible and Limit as a proportion of loss (Function 5)</t>
   </si>
   <si>
-    <t>E_2</t>
-  </si>
-  <si>
     <t>Limit with Deductible as a proportion of Limit (Function 9)</t>
   </si>
   <si>
-    <t>F_1</t>
-  </si>
-  <si>
     <t>Limit only (Function 14)</t>
   </si>
   <si>
-    <t>G_1</t>
-  </si>
-  <si>
     <t>Implemented</t>
   </si>
   <si>
@@ -282,9 +243,6 @@
     <t>Deductible and limit as a proportion of loss</t>
   </si>
   <si>
-    <t>to do</t>
-  </si>
-  <si>
     <t>Oasis smoke test FM with L1 L2 allocrule 0 L3 allocrule 1</t>
   </si>
   <si>
@@ -307,6 +265,36 @@
   </si>
   <si>
     <t>Special condition sublimits, blanket policy deductible and multiple policy layers</t>
+  </si>
+  <si>
+    <t>fm13</t>
+  </si>
+  <si>
+    <t>Excess policies with shares</t>
+  </si>
+  <si>
+    <t>2,12</t>
+  </si>
+  <si>
+    <t>3,6</t>
+  </si>
+  <si>
+    <t>Limit as a proportion of loss (Function 15)</t>
+  </si>
+  <si>
+    <t>Deductible as a proportion of loss (Function 16)</t>
+  </si>
+  <si>
+    <t>fm14</t>
+  </si>
+  <si>
+    <t>fm15</t>
+  </si>
+  <si>
+    <t>Limit as a proportion of loss</t>
+  </si>
+  <si>
+    <t>Deductible as a proportion of loss</t>
   </si>
 </sst>
 </file>
@@ -378,7 +366,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -391,6 +379,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -673,10 +664,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:L17"/>
+  <dimension ref="B1:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -688,18 +679,18 @@
   <sheetData>
     <row r="1" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="I3" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="J3" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
@@ -722,16 +713,16 @@
         <v>11</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="L4" s="3"/>
     </row>
@@ -752,16 +743,16 @@
         <v>3</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="K5" s="5"/>
     </row>
@@ -782,16 +773,16 @@
         <v>3</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="K6" s="5"/>
     </row>
@@ -800,10 +791,10 @@
         <v>12</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>7</v>
@@ -812,27 +803,27 @@
         <v>3</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="D8" s="7">
         <v>0</v>
@@ -850,19 +841,19 @@
         <v>1</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="K8" s="5"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="D9" s="5">
         <v>0</v>
@@ -880,19 +871,19 @@
         <v>1</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="K9" s="5"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="D10" s="5">
         <v>0</v>
@@ -910,19 +901,19 @@
         <v>1</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="K10" s="5"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="D11" s="5">
         <v>0</v>
@@ -940,25 +931,25 @@
         <v>1</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="K11" s="5"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="F12" s="7">
         <v>2</v>
@@ -967,22 +958,22 @@
         <v>1</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="K12" s="5"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="D13" s="5">
         <v>0</v>
@@ -997,24 +988,24 @@
         <v>1</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="K13" s="7" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="D14" s="5">
         <v>0</v>
@@ -1029,24 +1020,24 @@
         <v>1</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="K14" s="7" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="D15" s="5">
         <v>0</v>
@@ -1064,21 +1055,21 @@
         <v>2</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="K15" s="7" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="D16" s="5">
         <v>0</v>
@@ -1096,21 +1087,21 @@
         <v>10</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="K16" s="7" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="D17" s="5">
         <v>0</v>
@@ -1122,13 +1113,109 @@
         <v>7</v>
       </c>
       <c r="I17" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="K17" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B18" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D18" s="5">
+        <v>0</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="F18" s="7">
+        <v>2</v>
+      </c>
+      <c r="G18" s="7">
+        <v>1</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="J18" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="K18" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D19" s="5">
+        <v>0</v>
+      </c>
+      <c r="E19" s="7">
+        <v>16</v>
+      </c>
+      <c r="F19" s="7">
+        <v>1</v>
+      </c>
+      <c r="G19" s="7">
+        <v>1</v>
+      </c>
+      <c r="H19" s="7">
+        <v>14</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="K19" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B20" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C20" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="J17" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="K17" s="7" t="s">
-        <v>81</v>
+      <c r="D20" s="5">
+        <v>0</v>
+      </c>
+      <c r="E20" s="7">
+        <v>15</v>
+      </c>
+      <c r="F20" s="7">
+        <v>1</v>
+      </c>
+      <c r="G20" s="7">
+        <v>1</v>
+      </c>
+      <c r="H20" s="7">
+        <v>13</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="K20" s="7" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1138,10 +1225,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:I24"/>
+  <dimension ref="B2:H24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1153,12 +1240,13 @@
     <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H2" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" s="3"/>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>17</v>
       </c>
@@ -1171,378 +1259,379 @@
       <c r="E3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="I3" s="1" t="s">
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="2">
+        <v>2</v>
+      </c>
+      <c r="D5" s="2">
+        <v>3</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="2">
+        <v>3</v>
+      </c>
+      <c r="D6" s="2">
+        <v>12</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="2">
+        <v>4</v>
+      </c>
+      <c r="D7" s="2">
+        <v>10</v>
+      </c>
+      <c r="E7" s="2">
+        <v>3</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="2">
+        <v>5</v>
+      </c>
+      <c r="D8" s="2">
+        <v>11</v>
+      </c>
+      <c r="E8" s="2">
+        <v>3</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="2">
+        <v>6</v>
+      </c>
+      <c r="D9" s="2">
+        <v>2</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="2">
+        <v>7</v>
+      </c>
+      <c r="D10" s="2">
+        <v>13</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="2">
+        <v>8</v>
+      </c>
+      <c r="D11" s="2">
+        <v>6</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="2">
+        <v>9</v>
+      </c>
+      <c r="D12" s="2">
+        <v>4</v>
+      </c>
+      <c r="E12" s="2">
+        <v>1</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="2">
+        <v>10</v>
+      </c>
+      <c r="D13" s="2">
+        <v>5</v>
+      </c>
+      <c r="E13" s="2">
+        <v>1</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="2">
+        <v>11</v>
+      </c>
+      <c r="D14" s="2">
+        <v>9</v>
+      </c>
+      <c r="E14" s="2">
+        <v>1</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="2">
+        <v>12</v>
+      </c>
+      <c r="D15" s="2">
+        <v>14</v>
+      </c>
+      <c r="E15" s="2">
+        <v>1</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C16" s="2">
+        <v>13</v>
+      </c>
+      <c r="D16" s="2">
+        <v>15</v>
+      </c>
+      <c r="E16" s="2">
+        <v>1</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C17" s="2">
+        <v>14</v>
+      </c>
+      <c r="D17" s="2">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="2">
-        <v>1</v>
-      </c>
-      <c r="E4" s="2">
-        <v>1</v>
-      </c>
-      <c r="F4" s="2">
-        <v>1</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="2">
-        <v>2</v>
-      </c>
-      <c r="E5" s="2">
-        <v>3</v>
-      </c>
-      <c r="F5" s="2">
-        <v>1</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="2">
-        <v>3</v>
-      </c>
-      <c r="E6" s="2">
-        <v>12</v>
-      </c>
-      <c r="F6" s="2">
-        <v>1</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="2">
-        <v>4</v>
-      </c>
-      <c r="E7" s="2">
-        <v>10</v>
-      </c>
-      <c r="F7" s="2">
-        <v>3</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="2">
-        <v>5</v>
-      </c>
-      <c r="E8" s="2">
-        <v>11</v>
-      </c>
-      <c r="F8" s="2">
-        <v>3</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" s="2" t="s">
+      <c r="E17" s="2">
+        <v>1</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G18" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="2">
-        <v>6</v>
-      </c>
-      <c r="E9" s="2">
-        <v>2</v>
-      </c>
-      <c r="F9" s="2">
-        <v>1</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="H19" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="D10" s="2">
-        <v>7</v>
-      </c>
-      <c r="E10" s="2">
-        <v>13</v>
-      </c>
-      <c r="F10" s="2">
-        <v>1</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11" s="2">
-        <v>8</v>
-      </c>
-      <c r="E11" s="2">
-        <v>6</v>
-      </c>
-      <c r="F11" s="2">
-        <v>1</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D12" s="2">
-        <v>9</v>
-      </c>
-      <c r="E12" s="2">
-        <v>4</v>
-      </c>
-      <c r="F12" s="2">
-        <v>1</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" s="2">
-        <v>10</v>
-      </c>
-      <c r="E13" s="2">
-        <v>5</v>
-      </c>
-      <c r="F13" s="2">
-        <v>1</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D14" s="2">
-        <v>11</v>
-      </c>
-      <c r="E14" s="2">
-        <v>9</v>
-      </c>
-      <c r="F14" s="2">
-        <v>1</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D15" s="2">
-        <v>12</v>
-      </c>
-      <c r="E15" s="2">
-        <v>14</v>
-      </c>
-      <c r="F15" s="2">
-        <v>1</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H18" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B20" s="2" t="s">
-        <v>48</v>
       </c>
       <c r="C20" s="2">
         <v>-1</v>
       </c>
+      <c r="G20" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="H20" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I20" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="C21" s="2">
         <v>0</v>
       </c>
+      <c r="G21" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="H21" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I21" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="C22" s="2">
         <v>1</v>
       </c>
+      <c r="G22" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="H22" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="C23" s="2">
         <v>2</v>
       </c>
+      <c r="G23" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H23" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I23" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="C24" s="2">
         <v>3</v>
       </c>
+      <c r="G24" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H24" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I24" s="2" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added fm16 deductibles as percentage of limit
</commit_message>
<xml_diff>
--- a/ftest/ftest.xlsx
+++ b/ftest/ftest.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="93">
   <si>
     <t>yes</t>
   </si>
@@ -249,9 +249,6 @@
     <t>0,0,1</t>
   </si>
   <si>
-    <t>in progress</t>
-  </si>
-  <si>
     <t>Location deductibles with overall maximum policy deductible, and policy limit</t>
   </si>
   <si>
@@ -264,9 +261,6 @@
     <t>fm12</t>
   </si>
   <si>
-    <t>Special condition sublimits, blanket policy deductible and multiple policy layers</t>
-  </si>
-  <si>
     <t>fm13</t>
   </si>
   <si>
@@ -295,13 +289,28 @@
   </si>
   <si>
     <t>Deductible as a proportion of loss</t>
+  </si>
+  <si>
+    <t>fm16</t>
+  </si>
+  <si>
+    <t>Limit and Deductible as a proportion of limit</t>
+  </si>
+  <si>
+    <t>2,11,12,14</t>
+  </si>
+  <si>
+    <t>3,5,6,12</t>
+  </si>
+  <si>
+    <t>Special condition sublimits, blanket policy deductible and multiple policy layers, with and without back-allocation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -326,6 +335,13 @@
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -366,7 +382,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -384,6 +400,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -664,15 +682,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:L20"/>
+  <dimension ref="B1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="69.42578125" customWidth="1"/>
+    <col min="3" max="3" width="101.5703125" customWidth="1"/>
     <col min="9" max="10" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -809,10 +827,10 @@
         <v>42</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="K7" s="7" t="s">
         <v>68</v>
@@ -973,7 +991,7 @@
         <v>64</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D13" s="5">
         <v>0</v>
@@ -1005,7 +1023,7 @@
         <v>66</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D14" s="5">
         <v>0</v>
@@ -1037,7 +1055,7 @@
         <v>69</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D15" s="5">
         <v>0</v>
@@ -1098,13 +1116,16 @@
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="D17" s="5">
         <v>0</v>
+      </c>
+      <c r="E17" t="s">
+        <v>90</v>
       </c>
       <c r="F17" s="7">
         <v>6</v>
@@ -1112,11 +1133,14 @@
       <c r="G17" s="7">
         <v>7</v>
       </c>
+      <c r="H17" s="7" t="s">
+        <v>91</v>
+      </c>
       <c r="I17" s="5" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="K17" s="7" t="s">
         <v>68</v>
@@ -1124,16 +1148,16 @@
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D18" s="5">
+        <v>0</v>
+      </c>
+      <c r="E18" s="8" t="s">
         <v>80</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="D18" s="5">
-        <v>0</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>82</v>
       </c>
       <c r="F18" s="7">
         <v>2</v>
@@ -1142,7 +1166,7 @@
         <v>1</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I18" s="5" t="s">
         <v>65</v>
@@ -1156,10 +1180,10 @@
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D19" s="5">
         <v>0</v>
@@ -1188,10 +1212,10 @@
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D20" s="5">
         <v>0</v>
@@ -1215,6 +1239,38 @@
         <v>65</v>
       </c>
       <c r="K20" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B21" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D21" s="5">
+        <v>0</v>
+      </c>
+      <c r="E21" s="7">
+        <v>9</v>
+      </c>
+      <c r="F21" s="7">
+        <v>1</v>
+      </c>
+      <c r="G21" s="7">
+        <v>1</v>
+      </c>
+      <c r="H21" s="7">
+        <v>11</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="J21" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="K21" s="7" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1228,7 +1284,7 @@
   <dimension ref="B2:H24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1337,7 +1393,7 @@
         <v>10</v>
       </c>
       <c r="E7" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>1</v>
@@ -1357,7 +1413,7 @@
         <v>11</v>
       </c>
       <c r="E8" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>1</v>
@@ -1386,63 +1442,63 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
+    <row r="10" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="9">
         <v>7</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="9">
         <v>13</v>
       </c>
-      <c r="E10" s="2">
-        <v>1</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="2" t="s">
+      <c r="E10" s="9">
+        <v>1</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="9">
         <v>8</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="9">
         <v>6</v>
       </c>
-      <c r="E11" s="2">
-        <v>1</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="s">
+      <c r="E11" s="9">
+        <v>1</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="9">
         <v>9</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="9">
         <v>4</v>
       </c>
-      <c r="E12" s="2">
-        <v>1</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H12" s="2" t="s">
+      <c r="E12" s="9">
+        <v>1</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="H12" s="9" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1508,7 +1564,7 @@
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C16" s="2">
         <v>13</v>
@@ -1528,7 +1584,7 @@
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C17" s="2">
         <v>14</v>
@@ -1607,31 +1663,31 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="2" t="s">
+    <row r="23" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="9">
         <v>2</v>
       </c>
-      <c r="G23" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="2" t="s">
+      <c r="G23" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="H23" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24" s="9">
         <v>3</v>
       </c>
-      <c r="G24" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H24" s="2" t="s">
+      <c r="G24" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="H24" s="9" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added fm17 and 18 to test different allocrules. Not in runtests yet
</commit_message>
<xml_diff>
--- a/ftest/ftest.xlsx
+++ b/ftest/ftest.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\Joh\testgit\ktest\ftest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\Joh\testgit\ktest4\ftest\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="11025"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="11030"/>
   </bookViews>
   <sheets>
     <sheet name="ftests" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="99">
   <si>
     <t>yes</t>
   </si>
@@ -304,12 +304,30 @@
   </si>
   <si>
     <t>Special condition sublimits, blanket policy deductible and multiple policy layers, with and without back-allocation</t>
+  </si>
+  <si>
+    <t>fm17</t>
+  </si>
+  <si>
+    <t>-1,1</t>
+  </si>
+  <si>
+    <t>fm18</t>
+  </si>
+  <si>
+    <t>-1,2</t>
+  </si>
+  <si>
+    <t>WE5 Residential policy with coverage deductibles and blanket policy terms. Ground up loss back-allocation</t>
+  </si>
+  <si>
+    <t>WE5 Residential policy with coverage deductibles and blanket policy terms. Previous level input loss back-allocation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -682,25 +700,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:L21"/>
+  <dimension ref="B1:L23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="101.5703125" customWidth="1"/>
-    <col min="9" max="10" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="101.54296875" customWidth="1"/>
+    <col min="9" max="10" width="22.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.35">
       <c r="D3" t="s">
         <v>45</v>
       </c>
@@ -711,7 +729,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
@@ -744,7 +762,7 @@
       </c>
       <c r="L4" s="3"/>
     </row>
-    <row r="5" spans="2:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B5" s="5" t="s">
         <v>8</v>
       </c>
@@ -774,7 +792,7 @@
       </c>
       <c r="K5" s="5"/>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B6" s="5" t="s">
         <v>4</v>
       </c>
@@ -804,7 +822,7 @@
       </c>
       <c r="K6" s="5"/>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B7" s="5" t="s">
         <v>12</v>
       </c>
@@ -836,7 +854,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B8" s="5" t="s">
         <v>48</v>
       </c>
@@ -866,7 +884,7 @@
       </c>
       <c r="K8" s="5"/>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B9" s="5" t="s">
         <v>53</v>
       </c>
@@ -896,7 +914,7 @@
       </c>
       <c r="K9" s="5"/>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B10" s="5" t="s">
         <v>55</v>
       </c>
@@ -926,7 +944,7 @@
       </c>
       <c r="K10" s="5"/>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B11" s="5" t="s">
         <v>57</v>
       </c>
@@ -956,7 +974,7 @@
       </c>
       <c r="K11" s="5"/>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B12" s="5" t="s">
         <v>59</v>
       </c>
@@ -986,7 +1004,7 @@
       </c>
       <c r="K12" s="5"/>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B13" s="5" t="s">
         <v>64</v>
       </c>
@@ -1018,7 +1036,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B14" s="5" t="s">
         <v>66</v>
       </c>
@@ -1050,7 +1068,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B15" s="5" t="s">
         <v>69</v>
       </c>
@@ -1082,7 +1100,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B16" s="5" t="s">
         <v>70</v>
       </c>
@@ -1114,7 +1132,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B17" s="5" t="s">
         <v>77</v>
       </c>
@@ -1146,7 +1164,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B18" s="5" t="s">
         <v>78</v>
       </c>
@@ -1178,7 +1196,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B19" s="5" t="s">
         <v>84</v>
       </c>
@@ -1210,7 +1228,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B20" s="5" t="s">
         <v>85</v>
       </c>
@@ -1242,7 +1260,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B21" s="5" t="s">
         <v>88</v>
       </c>
@@ -1272,6 +1290,54 @@
       </c>
       <c r="K21" s="7" t="s">
         <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B22" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="F22" s="7">
+        <v>2</v>
+      </c>
+      <c r="G22" s="7">
+        <v>1</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B23" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="F23" s="7">
+        <v>2</v>
+      </c>
+      <c r="G23" s="7">
+        <v>1</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1287,22 +1353,22 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="61.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.26953125" customWidth="1"/>
+    <col min="5" max="5" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.35">
       <c r="G2" s="3" t="s">
         <v>33</v>
       </c>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
         <v>17</v>
       </c>
@@ -1322,7 +1388,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
         <v>21</v>
       </c>
@@ -1342,7 +1408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
         <v>22</v>
       </c>
@@ -1362,7 +1428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B6" s="2" t="s">
         <v>23</v>
       </c>
@@ -1382,7 +1448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B7" s="2" t="s">
         <v>24</v>
       </c>
@@ -1402,7 +1468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B8" s="2" t="s">
         <v>25</v>
       </c>
@@ -1422,7 +1488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B9" s="2" t="s">
         <v>26</v>
       </c>
@@ -1442,7 +1508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B10" s="9" t="s">
         <v>27</v>
       </c>
@@ -1462,7 +1528,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B11" s="9" t="s">
         <v>28</v>
       </c>
@@ -1482,7 +1548,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B12" s="9" t="s">
         <v>29</v>
       </c>
@@ -1502,7 +1568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B13" s="2" t="s">
         <v>30</v>
       </c>
@@ -1522,7 +1588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B14" s="2" t="s">
         <v>31</v>
       </c>
@@ -1542,7 +1608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B15" s="2" t="s">
         <v>32</v>
       </c>
@@ -1562,7 +1628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B16" s="2" t="s">
         <v>82</v>
       </c>
@@ -1582,7 +1648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B17" s="2" t="s">
         <v>83</v>
       </c>
@@ -1602,12 +1668,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.35">
       <c r="G18" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B19" s="1" t="s">
         <v>40</v>
       </c>
@@ -1621,7 +1687,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B20" s="2" t="s">
         <v>35</v>
       </c>
@@ -1635,7 +1701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B21" s="2" t="s">
         <v>36</v>
       </c>
@@ -1649,7 +1715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B22" s="2" t="s">
         <v>37</v>
       </c>
@@ -1663,7 +1729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B23" s="9" t="s">
         <v>38</v>
       </c>
@@ -1677,7 +1743,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B24" s="9" t="s">
         <v>39</v>
       </c>

</xml_diff>

<commit_message>
added fm19 to test allocrule 2
</commit_message>
<xml_diff>
--- a/ftest/ftest.xlsx
+++ b/ftest/ftest.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17766"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\Joh\testgit\ktest4\ftest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\Joh\testgit\ktest\ftest\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="11030"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="11028"/>
   </bookViews>
   <sheets>
     <sheet name="ftests" sheetId="1" r:id="rId1"/>
     <sheet name="test parameters" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="101">
   <si>
     <t>yes</t>
   </si>
@@ -309,19 +309,25 @@
     <t>fm17</t>
   </si>
   <si>
-    <t>-1,1</t>
-  </si>
-  <si>
     <t>fm18</t>
   </si>
   <si>
-    <t>-1,2</t>
-  </si>
-  <si>
     <t>WE5 Residential policy with coverage deductibles and blanket policy terms. Ground up loss back-allocation</t>
   </si>
   <si>
     <t>WE5 Residential policy with coverage deductibles and blanket policy terms. Previous level input loss back-allocation</t>
+  </si>
+  <si>
+    <t>fm19</t>
+  </si>
+  <si>
+    <t>0,1</t>
+  </si>
+  <si>
+    <t>0,2</t>
+  </si>
+  <si>
+    <t>Residential policy with blanket policy terms. Previous level input loss back-allocation</t>
   </si>
 </sst>
 </file>
@@ -700,25 +706,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:L23"/>
+  <dimension ref="B1:L24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="101.54296875" customWidth="1"/>
-    <col min="9" max="10" width="22.81640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="101.5546875" customWidth="1"/>
+    <col min="9" max="10" width="22.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
       <c r="D3" t="s">
         <v>45</v>
       </c>
@@ -729,7 +735,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
@@ -762,7 +768,7 @@
       </c>
       <c r="L4" s="3"/>
     </row>
-    <row r="5" spans="2:12" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B5" s="5" t="s">
         <v>8</v>
       </c>
@@ -792,7 +798,7 @@
       </c>
       <c r="K5" s="5"/>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B6" s="5" t="s">
         <v>4</v>
       </c>
@@ -822,7 +828,7 @@
       </c>
       <c r="K6" s="5"/>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B7" s="5" t="s">
         <v>12</v>
       </c>
@@ -854,7 +860,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B8" s="5" t="s">
         <v>48</v>
       </c>
@@ -884,7 +890,7 @@
       </c>
       <c r="K8" s="5"/>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B9" s="5" t="s">
         <v>53</v>
       </c>
@@ -914,7 +920,7 @@
       </c>
       <c r="K9" s="5"/>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B10" s="5" t="s">
         <v>55</v>
       </c>
@@ -944,7 +950,7 @@
       </c>
       <c r="K10" s="5"/>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B11" s="5" t="s">
         <v>57</v>
       </c>
@@ -974,7 +980,7 @@
       </c>
       <c r="K11" s="5"/>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B12" s="5" t="s">
         <v>59</v>
       </c>
@@ -1004,7 +1010,7 @@
       </c>
       <c r="K12" s="5"/>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B13" s="5" t="s">
         <v>64</v>
       </c>
@@ -1036,7 +1042,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B14" s="5" t="s">
         <v>66</v>
       </c>
@@ -1068,7 +1074,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B15" s="5" t="s">
         <v>69</v>
       </c>
@@ -1100,7 +1106,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B16" s="5" t="s">
         <v>70</v>
       </c>
@@ -1132,7 +1138,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B17" s="5" t="s">
         <v>77</v>
       </c>
@@ -1164,7 +1170,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B18" s="5" t="s">
         <v>78</v>
       </c>
@@ -1196,7 +1202,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B19" s="5" t="s">
         <v>84</v>
       </c>
@@ -1228,7 +1234,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B20" s="5" t="s">
         <v>85</v>
       </c>
@@ -1260,7 +1266,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B21" s="5" t="s">
         <v>88</v>
       </c>
@@ -1292,15 +1298,15 @@
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B22" s="5" t="s">
         <v>93</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="E22" s="7" t="s">
         <v>61</v>
@@ -1317,15 +1323,15 @@
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B23" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>61</v>
@@ -1338,6 +1344,29 @@
       </c>
       <c r="H23" s="7" t="s">
         <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B24" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D24" s="5">
+        <v>2</v>
+      </c>
+      <c r="E24" s="7">
+        <v>1</v>
+      </c>
+      <c r="F24" s="7">
+        <v>1</v>
+      </c>
+      <c r="G24" s="7">
+        <v>1</v>
+      </c>
+      <c r="H24" s="7">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1353,22 +1382,22 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="61.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.26953125" customWidth="1"/>
-    <col min="5" max="5" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.21875" customWidth="1"/>
+    <col min="5" max="5" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
       <c r="G2" s="3" t="s">
         <v>33</v>
       </c>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>17</v>
       </c>
@@ -1388,7 +1417,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>21</v>
       </c>
@@ -1408,7 +1437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>22</v>
       </c>
@@ -1428,7 +1457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>23</v>
       </c>
@@ -1448,7 +1477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
         <v>24</v>
       </c>
@@ -1468,7 +1497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
         <v>25</v>
       </c>
@@ -1488,7 +1517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>26</v>
       </c>
@@ -1508,7 +1537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B10" s="9" t="s">
         <v>27</v>
       </c>
@@ -1528,7 +1557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B11" s="9" t="s">
         <v>28</v>
       </c>
@@ -1548,7 +1577,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B12" s="9" t="s">
         <v>29</v>
       </c>
@@ -1568,7 +1597,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
         <v>30</v>
       </c>
@@ -1588,7 +1617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>31</v>
       </c>
@@ -1608,7 +1637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
         <v>32</v>
       </c>
@@ -1628,7 +1657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="s">
         <v>82</v>
       </c>
@@ -1648,7 +1677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
         <v>83</v>
       </c>
@@ -1668,12 +1697,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
       <c r="G18" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
         <v>40</v>
       </c>
@@ -1687,7 +1716,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B20" s="2" t="s">
         <v>35</v>
       </c>
@@ -1701,7 +1730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B21" s="2" t="s">
         <v>36</v>
       </c>
@@ -1715,7 +1744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B22" s="2" t="s">
         <v>37</v>
       </c>
@@ -1729,7 +1758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B23" s="9" t="s">
         <v>38</v>
       </c>
@@ -1743,7 +1772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B24" s="9" t="s">
         <v>39</v>
       </c>

</xml_diff>

<commit_message>
completed ftests 17 18 19
</commit_message>
<xml_diff>
--- a/ftest/ftest.xlsx
+++ b/ftest/ftest.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\Joh\testgit\ktest\ftest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\Joh\git\ktest2\ftest\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="11028"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="11030"/>
   </bookViews>
   <sheets>
     <sheet name="ftests" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="101">
   <si>
     <t>yes</t>
   </si>
@@ -709,22 +709,22 @@
   <dimension ref="B1:L24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="101.5546875" customWidth="1"/>
-    <col min="9" max="10" width="22.77734375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="101.54296875" customWidth="1"/>
+    <col min="9" max="10" width="22.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.35">
       <c r="D3" t="s">
         <v>45</v>
       </c>
@@ -735,7 +735,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
@@ -768,7 +768,7 @@
       </c>
       <c r="L4" s="3"/>
     </row>
-    <row r="5" spans="2:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:12" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B5" s="5" t="s">
         <v>8</v>
       </c>
@@ -798,7 +798,7 @@
       </c>
       <c r="K5" s="5"/>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B6" s="5" t="s">
         <v>4</v>
       </c>
@@ -828,7 +828,7 @@
       </c>
       <c r="K6" s="5"/>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B7" s="5" t="s">
         <v>12</v>
       </c>
@@ -860,7 +860,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B8" s="5" t="s">
         <v>48</v>
       </c>
@@ -890,7 +890,7 @@
       </c>
       <c r="K8" s="5"/>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B9" s="5" t="s">
         <v>53</v>
       </c>
@@ -920,7 +920,7 @@
       </c>
       <c r="K9" s="5"/>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B10" s="5" t="s">
         <v>55</v>
       </c>
@@ -950,7 +950,7 @@
       </c>
       <c r="K10" s="5"/>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B11" s="5" t="s">
         <v>57</v>
       </c>
@@ -980,7 +980,7 @@
       </c>
       <c r="K11" s="5"/>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B12" s="5" t="s">
         <v>59</v>
       </c>
@@ -1010,7 +1010,7 @@
       </c>
       <c r="K12" s="5"/>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B13" s="5" t="s">
         <v>64</v>
       </c>
@@ -1042,7 +1042,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B14" s="5" t="s">
         <v>66</v>
       </c>
@@ -1074,7 +1074,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B15" s="5" t="s">
         <v>69</v>
       </c>
@@ -1106,7 +1106,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B16" s="5" t="s">
         <v>70</v>
       </c>
@@ -1138,7 +1138,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B17" s="5" t="s">
         <v>77</v>
       </c>
@@ -1170,7 +1170,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B18" s="5" t="s">
         <v>78</v>
       </c>
@@ -1202,7 +1202,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B19" s="5" t="s">
         <v>84</v>
       </c>
@@ -1234,7 +1234,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B20" s="5" t="s">
         <v>85</v>
       </c>
@@ -1266,7 +1266,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B21" s="5" t="s">
         <v>88</v>
       </c>
@@ -1298,7 +1298,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B22" s="5" t="s">
         <v>93</v>
       </c>
@@ -1320,10 +1320,17 @@
       <c r="H22" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="I22" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="J22" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="K22" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B23" s="5" t="s">
         <v>94</v>
       </c>
@@ -1345,8 +1352,17 @@
       <c r="H23" s="7" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="I23" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="J23" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="K23" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B24" s="5" t="s">
         <v>97</v>
       </c>
@@ -1367,6 +1383,15 @@
       </c>
       <c r="H24" s="7">
         <v>1</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="J24" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="K24" s="7" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1382,22 +1407,22 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="61.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.21875" customWidth="1"/>
-    <col min="5" max="5" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1796875" customWidth="1"/>
+    <col min="5" max="5" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.35">
       <c r="G2" s="3" t="s">
         <v>33</v>
       </c>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
         <v>17</v>
       </c>
@@ -1417,7 +1442,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
         <v>21</v>
       </c>
@@ -1437,7 +1462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
         <v>22</v>
       </c>
@@ -1457,7 +1482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B6" s="2" t="s">
         <v>23</v>
       </c>
@@ -1477,7 +1502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B7" s="2" t="s">
         <v>24</v>
       </c>
@@ -1497,7 +1522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B8" s="2" t="s">
         <v>25</v>
       </c>
@@ -1517,7 +1542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B9" s="2" t="s">
         <v>26</v>
       </c>
@@ -1537,7 +1562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B10" s="9" t="s">
         <v>27</v>
       </c>
@@ -1557,7 +1582,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B11" s="9" t="s">
         <v>28</v>
       </c>
@@ -1577,7 +1602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B12" s="9" t="s">
         <v>29</v>
       </c>
@@ -1597,7 +1622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B13" s="2" t="s">
         <v>30</v>
       </c>
@@ -1617,7 +1642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B14" s="2" t="s">
         <v>31</v>
       </c>
@@ -1637,7 +1662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B15" s="2" t="s">
         <v>32</v>
       </c>
@@ -1657,7 +1682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B16" s="2" t="s">
         <v>82</v>
       </c>
@@ -1677,7 +1702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B17" s="2" t="s">
         <v>83</v>
       </c>
@@ -1697,12 +1722,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.35">
       <c r="G18" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B19" s="1" t="s">
         <v>40</v>
       </c>
@@ -1716,7 +1741,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B20" s="2" t="s">
         <v>35</v>
       </c>
@@ -1730,7 +1755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B21" s="2" t="s">
         <v>36</v>
       </c>
@@ -1744,7 +1769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B22" s="2" t="s">
         <v>37</v>
       </c>
@@ -1758,7 +1783,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B23" s="9" t="s">
         <v>38</v>
       </c>
@@ -1772,7 +1797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B24" s="9" t="s">
         <v>39</v>
       </c>

</xml_diff>

<commit_message>
added test fm21 wip
</commit_message>
<xml_diff>
--- a/ftest/ftest.xlsx
+++ b/ftest/ftest.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="105">
   <si>
     <t>yes</t>
   </si>
@@ -331,6 +331,15 @@
   </si>
   <si>
     <t>Special condition sublimits, blanket policy deductible and multiple policy layers</t>
+  </si>
+  <si>
+    <t>fm21</t>
+  </si>
+  <si>
+    <t>Location deductibles with overall maximum policy deductible, and policy limit with IL back-allocation</t>
+  </si>
+  <si>
+    <t>wip</t>
   </si>
 </sst>
 </file>
@@ -709,10 +718,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:L25"/>
+  <dimension ref="B1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1398,6 +1407,35 @@
       </c>
       <c r="J25" s="5" t="s">
         <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B26" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="E26" s="7">
+        <v>10</v>
+      </c>
+      <c r="F26" s="7">
+        <v>3</v>
+      </c>
+      <c r="G26" s="7">
+        <v>1</v>
+      </c>
+      <c r="H26" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="J26" s="5" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
completed fm21 and fm22 for allocrule 2 testing
</commit_message>
<xml_diff>
--- a/ftest/ftest.xlsx
+++ b/ftest/ftest.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="106">
   <si>
     <t>yes</t>
   </si>
@@ -339,7 +339,10 @@
     <t>Location deductibles with overall maximum policy deductible, and policy limit with IL back-allocation</t>
   </si>
   <si>
-    <t>wip</t>
+    <t>fm22</t>
+  </si>
+  <si>
+    <t>Special condition sublimits, blanket policy deductible and multiple policy layers, with IL back-allocation</t>
   </si>
 </sst>
 </file>
@@ -718,10 +721,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:L26"/>
+  <dimension ref="B1:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1432,10 +1435,39 @@
         <v>67</v>
       </c>
       <c r="I26" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="J26" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B27" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="J26" s="5" t="s">
-        <v>104</v>
+      <c r="C27" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D27" t="s">
+        <v>97</v>
+      </c>
+      <c r="E27" t="s">
+        <v>89</v>
+      </c>
+      <c r="F27" s="7">
+        <v>6</v>
+      </c>
+      <c r="G27" s="7">
+        <v>7</v>
+      </c>
+      <c r="H27" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="J27" s="5" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added checksums for fm23 and fm24
</commit_message>
<xml_diff>
--- a/ftest/ftest.xlsx
+++ b/ftest/ftest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\Joh\git\ktest\ftest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{F1F7BA72-81A2-4A39-B301-832D53DF0734}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{171ABCB9-14A4-49F2-9EEA-80B2FC896DD0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="11028" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -370,13 +370,13 @@
     <t>fm26</t>
   </si>
   <si>
-    <t>Third iteration of fm25 - 2 layers at level 1 and apply occurrence cap at level 2, gross perspective</t>
-  </si>
-  <si>
     <t>fm27</t>
   </si>
   <si>
     <t>fm 26 in two iterations, gross perspective</t>
+  </si>
+  <si>
+    <t>Third iteration of fm24 - 2 layers at level 1 and apply occurrence cap at level 2, gross perspective</t>
   </si>
 </sst>
 </file>
@@ -758,7 +758,7 @@
   <dimension ref="B1:L32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1551,7 +1551,7 @@
         <v>113</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="I31" s="5" t="s">
         <v>111</v>
@@ -1562,10 +1562,10 @@
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B32" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C32" s="5" t="s">
         <v>115</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>116</v>
       </c>
       <c r="I32" s="5" t="s">
         <v>111</v>

</xml_diff>

<commit_message>
added test for %tiv deductibles
</commit_message>
<xml_diff>
--- a/ftest/ftest.xlsx
+++ b/ftest/ftest.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\Joh\git\ktest2\ftest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\Joh\git\ktest\ftest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{FA80E2BB-7FE2-42DF-89B2-B1F2060728B2}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{8447DADB-0C7A-46FA-9D38-7211D3271F5B}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="11028" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="113">
   <si>
     <t>yes</t>
   </si>
@@ -362,6 +362,9 @@
   </si>
   <si>
     <t>Special condition sublimits, blanket policy deductible and multiple policy layers, with prior level back-allocation</t>
+  </si>
+  <si>
+    <t>Direct level from fm24 testing % TIV deductibles</t>
   </si>
 </sst>
 </file>
@@ -742,7 +745,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
@@ -1470,9 +1473,27 @@
       <c r="B30" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="C30" s="5"/>
-      <c r="H30" s="5"/>
-      <c r="I30" s="5"/>
+      <c r="C30" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D30">
+        <v>2</v>
+      </c>
+      <c r="E30">
+        <v>4</v>
+      </c>
+      <c r="F30" s="7">
+        <v>2</v>
+      </c>
+      <c r="G30" s="7">
+        <v>1</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="I30" s="5" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B31" s="5" t="s">

</xml_diff>

<commit_message>
added fm26 test for calcrule 6
</commit_message>
<xml_diff>
--- a/ftest/ftest.xlsx
+++ b/ftest/ftest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\Joh\git\ktest\ftest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{8447DADB-0C7A-46FA-9D38-7211D3271F5B}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{2C595E08-A9B9-4155-97C2-59D5BB21F4EA}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="11028" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="114">
   <si>
     <t>yes</t>
   </si>
@@ -364,7 +364,10 @@
     <t>Special condition sublimits, blanket policy deductible and multiple policy layers, with prior level back-allocation</t>
   </si>
   <si>
-    <t>Direct level from fm24 testing % TIV deductibles</t>
+    <t>Direct level from fm24 testing % TIV deductibles calcrule 6</t>
+  </si>
+  <si>
+    <t>Direct level from fm24 testing % TIV deductibles with limits calcrule 4</t>
   </si>
 </sst>
 </file>
@@ -746,7 +749,7 @@
   <dimension ref="B1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1474,7 +1477,7 @@
         <v>102</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D30">
         <v>2</v>
@@ -1499,9 +1502,27 @@
       <c r="B31" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="C31" s="5"/>
-      <c r="H31" s="5"/>
-      <c r="I31" s="5"/>
+      <c r="C31" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D31">
+        <v>2</v>
+      </c>
+      <c r="E31">
+        <v>6</v>
+      </c>
+      <c r="F31" s="7">
+        <v>2</v>
+      </c>
+      <c r="G31" s="7">
+        <v>1</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="I31" s="5" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B32" s="5" t="s">

</xml_diff>

<commit_message>
seperated fac from surplus share by adding ri1a for fac
</commit_message>
<xml_diff>
--- a/ftest/ftest.xlsx
+++ b/ftest/ftest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\Joh\git\ktest\ftest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{2C595E08-A9B9-4155-97C2-59D5BB21F4EA}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C5894451-2BFF-4AC5-A6C1-C13EF4F739F0}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="11028" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="116">
   <si>
     <t>yes</t>
   </si>
@@ -368,6 +368,12 @@
   </si>
   <si>
     <t>Direct level from fm24 testing % TIV deductibles with limits calcrule 4</t>
+  </si>
+  <si>
+    <t>14,21, 23,25</t>
+  </si>
+  <si>
+    <t>Reinsurance example with location level fac and surplus share on a subset of locations and two per risk treaties on all locations</t>
   </si>
 </sst>
 </file>
@@ -1492,10 +1498,10 @@
         <v>1</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>101</v>
+        <v>62</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>101</v>
+        <v>62</v>
       </c>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.3">
@@ -1518,19 +1524,37 @@
         <v>1</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>101</v>
+        <v>62</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>101</v>
+        <v>62</v>
       </c>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B32" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="C32" s="5"/>
-      <c r="H32" s="5"/>
-      <c r="I32" s="5"/>
+      <c r="C32" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D32" t="s">
+        <v>90</v>
+      </c>
+      <c r="E32" t="s">
+        <v>114</v>
+      </c>
+      <c r="F32" s="7">
+        <v>2</v>
+      </c>
+      <c r="G32" s="7">
+        <v>2</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="I32" s="5" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B33" s="5" t="s">

</xml_diff>

<commit_message>
completed fm27 except reorg
</commit_message>
<xml_diff>
--- a/ftest/ftest.xlsx
+++ b/ftest/ftest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\Joh\git\ktest\ftest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C5894451-2BFF-4AC5-A6C1-C13EF4F739F0}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{DF425DEE-BE99-4BBD-AED1-627CB54783C4}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="11028" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -755,7 +755,7 @@
   <dimension ref="B1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1550,10 +1550,10 @@
         <v>2</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>101</v>
+        <v>62</v>
       </c>
       <c r="I32" s="5" t="s">
-        <v>101</v>
+        <v>62</v>
       </c>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
added tests for calcrule 7 and 8
</commit_message>
<xml_diff>
--- a/ftest/ftest.xlsx
+++ b/ftest/ftest.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\Joh\git\ktest\ftest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{DF425DEE-BE99-4BBD-AED1-627CB54783C4}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{51DF672C-26AF-4E2C-B4CB-7BB3372E8DEB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="11028" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="ftests" sheetId="1" r:id="rId1"/>
     <sheet name="test parameters" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="122">
   <si>
     <t>yes</t>
   </si>
@@ -301,9 +301,6 @@
     <t>0,2</t>
   </si>
   <si>
-    <t>Residential policy with blanket policy terms. Previous level input loss back-allocation</t>
-  </si>
-  <si>
     <t>fm20</t>
   </si>
   <si>
@@ -374,6 +371,27 @@
   </si>
   <si>
     <t>Reinsurance example with location level fac and surplus share on a subset of locations and two per risk treaties on all locations</t>
+  </si>
+  <si>
+    <t>Residential policy with blanket policy terms. Prior level loss back-allocation</t>
+  </si>
+  <si>
+    <t>fm29</t>
+  </si>
+  <si>
+    <t>fm30</t>
+  </si>
+  <si>
+    <t>6,7</t>
+  </si>
+  <si>
+    <t>Location deductibles with overall maximum policy deductible, and policy limit using calcrules 6 &amp; 7</t>
+  </si>
+  <si>
+    <t>Location deductibles with overall minimum policy deductible, and policy limit using calcrule 6 &amp; 8</t>
+  </si>
+  <si>
+    <t>6,8</t>
   </si>
 </sst>
 </file>
@@ -752,10 +770,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:K33"/>
+  <dimension ref="B1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1140,7 +1158,7 @@
         <v>72</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D17" s="5">
         <v>0</v>
@@ -1302,7 +1320,7 @@
         <v>86</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>90</v>
@@ -1329,7 +1347,7 @@
         <v>88</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>91</v>
+        <v>115</v>
       </c>
       <c r="D24" s="5">
         <v>2</v>
@@ -1353,10 +1371,10 @@
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B25" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C25" s="5" t="s">
         <v>92</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>93</v>
       </c>
       <c r="D25" s="5">
         <v>1</v>
@@ -1379,10 +1397,10 @@
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B26" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D26" s="7" t="s">
         <v>90</v>
@@ -1405,10 +1423,10 @@
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B27" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D27" t="s">
         <v>90</v>
@@ -1431,16 +1449,16 @@
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B28" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C28" s="5" t="s">
         <v>97</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>98</v>
       </c>
       <c r="D28">
         <v>2</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F28" s="7">
         <v>2</v>
@@ -1457,16 +1475,16 @@
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B29" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C29" s="5" t="s">
         <v>99</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>100</v>
       </c>
       <c r="D29" t="s">
         <v>90</v>
       </c>
       <c r="E29" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G29" s="7">
         <v>5</v>
@@ -1480,10 +1498,10 @@
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B30" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D30">
         <v>2</v>
@@ -1506,10 +1524,10 @@
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B31" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D31">
         <v>2</v>
@@ -1532,16 +1550,16 @@
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B32" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D32" t="s">
         <v>90</v>
       </c>
       <c r="E32" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F32" s="7">
         <v>2</v>
@@ -1558,16 +1576,68 @@
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B33" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C33" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="C33" s="5" t="s">
-        <v>106</v>
-      </c>
       <c r="H33" s="5" t="s">
-        <v>101</v>
+        <v>62</v>
       </c>
       <c r="I33" s="5" t="s">
-        <v>101</v>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B34" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34" t="s">
+        <v>118</v>
+      </c>
+      <c r="F34" s="7">
+        <v>2</v>
+      </c>
+      <c r="G34" s="7">
+        <v>1</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="I34" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B35" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35" t="s">
+        <v>121</v>
+      </c>
+      <c r="F35" s="7">
+        <v>2</v>
+      </c>
+      <c r="G35" s="7">
+        <v>1</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="I35" s="5" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added test for min max deductibles calcrule 13
</commit_message>
<xml_diff>
--- a/ftest/ftest.xlsx
+++ b/ftest/ftest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\Joh\git\ktest\ftest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{51DF672C-26AF-4E2C-B4CB-7BB3372E8DEB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{4F2A1BB6-72A5-42A7-878E-B6BF20B549D5}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="11028" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="125">
   <si>
     <t>yes</t>
   </si>
@@ -392,6 +392,15 @@
   </si>
   <si>
     <t>6,8</t>
+  </si>
+  <si>
+    <t>fm31</t>
+  </si>
+  <si>
+    <t>Min and Max deductibles test calcrule 13</t>
+  </si>
+  <si>
+    <t>6, 13</t>
   </si>
 </sst>
 </file>
@@ -770,10 +779,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:K35"/>
+  <dimension ref="B1:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1608,10 +1617,10 @@
         <v>1</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>100</v>
+        <v>62</v>
       </c>
       <c r="I34" s="5" t="s">
-        <v>100</v>
+        <v>62</v>
       </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.3">
@@ -1634,9 +1643,35 @@
         <v>1</v>
       </c>
       <c r="H35" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I35" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B36" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36" t="s">
+        <v>124</v>
+      </c>
+      <c r="F36" s="7">
+        <v>2</v>
+      </c>
+      <c r="G36" s="7">
+        <v>1</v>
+      </c>
+      <c r="H36" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="I35" s="5" t="s">
+      <c r="I36" s="5" t="s">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
completed fm31 and fm34
</commit_message>
<xml_diff>
--- a/ftest/ftest.xlsx
+++ b/ftest/ftest.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\Joh\git\ktest\ftest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{336AB0F8-518C-4BA9-BA6A-7506B914D16B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{268E43F3-AE2E-41DF-9A90-A0B8BB4BAEEC}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="11028" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="130">
   <si>
     <t>yes</t>
   </si>
@@ -326,9 +326,6 @@
   </si>
   <si>
     <t>Complex reinsurance programme with 4 inuring levels</t>
-  </si>
-  <si>
-    <t>in progress</t>
   </si>
   <si>
     <t>fm25</t>
@@ -799,8 +796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:K39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1347,7 +1344,7 @@
         <v>86</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>90</v>
@@ -1374,7 +1371,7 @@
         <v>88</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D24" s="5">
         <v>2</v>
@@ -1427,7 +1424,7 @@
         <v>94</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D26" s="7" t="s">
         <v>90</v>
@@ -1453,7 +1450,7 @@
         <v>95</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D27" t="s">
         <v>90</v>
@@ -1485,7 +1482,7 @@
         <v>2</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F28" s="7">
         <v>2</v>
@@ -1511,7 +1508,7 @@
         <v>90</v>
       </c>
       <c r="E29" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G29" s="7">
         <v>5</v>
@@ -1525,10 +1522,10 @@
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B30" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D30">
         <v>2</v>
@@ -1551,10 +1548,10 @@
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B31" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D31">
         <v>2</v>
@@ -1577,16 +1574,16 @@
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B32" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D32" t="s">
         <v>90</v>
       </c>
       <c r="E32" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F32" s="7">
         <v>2</v>
@@ -1603,10 +1600,10 @@
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B33" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C33" s="5" t="s">
         <v>104</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>105</v>
       </c>
       <c r="H33" s="5" t="s">
         <v>62</v>
@@ -1617,16 +1614,16 @@
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B34" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D34">
         <v>0</v>
       </c>
       <c r="E34" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F34" s="7">
         <v>2</v>
@@ -1643,16 +1640,16 @@
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B35" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C35" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35" t="s">
         <v>120</v>
-      </c>
-      <c r="D35">
-        <v>0</v>
-      </c>
-      <c r="E35" t="s">
-        <v>121</v>
       </c>
       <c r="F35" s="7">
         <v>2</v>
@@ -1669,16 +1666,16 @@
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B36" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C36" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36" t="s">
         <v>123</v>
-      </c>
-      <c r="D36">
-        <v>0</v>
-      </c>
-      <c r="E36" t="s">
-        <v>124</v>
       </c>
       <c r="F36" s="7">
         <v>2</v>
@@ -1687,18 +1684,18 @@
         <v>1</v>
       </c>
       <c r="H36" s="5" t="s">
-        <v>100</v>
+        <v>62</v>
       </c>
       <c r="I36" s="5" t="s">
-        <v>100</v>
+        <v>62</v>
       </c>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B37" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C37" s="5" t="s">
         <v>125</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>126</v>
       </c>
       <c r="D37" s="5">
         <v>0</v>
@@ -1721,10 +1718,10 @@
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B38" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D38" s="5">
         <v>0</v>
@@ -1747,10 +1744,10 @@
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B39" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D39" s="5">
         <v>0</v>
@@ -1765,10 +1762,10 @@
         <v>1</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>100</v>
+        <v>62</v>
       </c>
       <c r="I39" s="5" t="s">
-        <v>100</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test for calcrule 19
</commit_message>
<xml_diff>
--- a/ftest/ftest.xlsx
+++ b/ftest/ftest.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\Joh\git\ktest\ftest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{268E43F3-AE2E-41DF-9A90-A0B8BB4BAEEC}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{B076E708-7735-42AA-9D55-D393D9474F57}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="11028" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="133">
   <si>
     <t>yes</t>
   </si>
@@ -416,6 +416,15 @@
   </si>
   <si>
     <t>Excess policies with shares and blanket deductible (% tiv) using calcrule 18</t>
+  </si>
+  <si>
+    <t>fm35</t>
+  </si>
+  <si>
+    <t>% Loss deductible with min and max deductible. Calcrule 19</t>
+  </si>
+  <si>
+    <t>in progress</t>
   </si>
 </sst>
 </file>
@@ -794,10 +803,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:K39"/>
+  <dimension ref="B1:K41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="D26" workbookViewId="0">
+      <selection activeCell="H40" sqref="H40:I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1767,6 +1776,35 @@
       <c r="I39" s="5" t="s">
         <v>62</v>
       </c>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B40" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D40" s="5">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>19</v>
+      </c>
+      <c r="F40" s="7">
+        <v>1</v>
+      </c>
+      <c r="G40" s="7">
+        <v>1</v>
+      </c>
+      <c r="H40" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="I40" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B41" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added quota share example calcrule 22
</commit_message>
<xml_diff>
--- a/ftest/ftest.xlsx
+++ b/ftest/ftest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\Joh\git\ktest\ftest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{51F1DBCC-3F49-423B-9C19-D00F9FC1BB5A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{AEFE5653-9A47-40C5-AB3C-866169FCAF61}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="11028" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="136">
   <si>
     <t>yes</t>
   </si>
@@ -422,6 +422,18 @@
   </si>
   <si>
     <t>% Loss deductible with min and max deductible. Calcrule 19</t>
+  </si>
+  <si>
+    <t>fm36</t>
+  </si>
+  <si>
+    <t>Reverse Franchise deductible calcrule 20</t>
+  </si>
+  <si>
+    <t>fm37</t>
+  </si>
+  <si>
+    <t>WE11 Quota Share with % placed and % treaty share for 2 Reinsurers</t>
   </si>
 </sst>
 </file>
@@ -800,9 +812,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:K41"/>
+  <dimension ref="B1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1799,7 +1813,56 @@
       </c>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B41" s="5"/>
+      <c r="B41" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D41" s="5">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>20</v>
+      </c>
+      <c r="F41" s="7">
+        <v>1</v>
+      </c>
+      <c r="G41" s="7">
+        <v>1</v>
+      </c>
+      <c r="H41" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I41" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B42" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="E42">
+        <v>22</v>
+      </c>
+      <c r="F42" s="7">
+        <v>2</v>
+      </c>
+      <c r="G42" s="7">
+        <v>2</v>
+      </c>
+      <c r="H42" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I42" s="5" t="s">
+        <v>62</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added test for another bug to fix
</commit_message>
<xml_diff>
--- a/ftest/ftest.xlsx
+++ b/ftest/ftest.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\Joh\git\ktest\ftest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{AEFE5653-9A47-40C5-AB3C-866169FCAF61}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{9A497F4A-F7B9-4427-BF79-8F27D1BFC7D8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="11028" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="141">
   <si>
     <t>yes</t>
   </si>
@@ -434,6 +434,21 @@
   </si>
   <si>
     <t>WE11 Quota Share with % placed and % treaty share for 2 Reinsurers</t>
+  </si>
+  <si>
+    <t>fm38</t>
+  </si>
+  <si>
+    <t>BugToFix: 3 CAT XL layers net loss error at level 3</t>
+  </si>
+  <si>
+    <t>fm39</t>
+  </si>
+  <si>
+    <t>BugToFix: fm24 inuring level 3 outputs wrong net loss when losses carried to level 3</t>
+  </si>
+  <si>
+    <t>in progress</t>
   </si>
 </sst>
 </file>
@@ -812,10 +827,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:K42"/>
+  <dimension ref="B1:K44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1862,6 +1877,34 @@
       </c>
       <c r="I42" s="5" t="s">
         <v>62</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B43" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="H43" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="I43" s="5" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B44" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="H44" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="I44" s="5" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated calcrule 19 tests to include effective deductibles
</commit_message>
<xml_diff>
--- a/ftest/ftest.xlsx
+++ b/ftest/ftest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\Joh\git\ktest\ftest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{076D5588-54FA-4187-8FA5-F9E232D241FC}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28F2D4CB-7D72-4344-AB68-21AF083927A9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="11028" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="11025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ftests" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="137">
   <si>
     <t>yes</t>
   </si>
@@ -400,9 +400,6 @@
     <t>fm35</t>
   </si>
   <si>
-    <t>% Loss deductible with min and max deductible. Calcrule 19</t>
-  </si>
-  <si>
     <t>fm36</t>
   </si>
   <si>
@@ -434,6 +431,12 @@
   </si>
   <si>
     <t>Location deductibles with overall maximum policy deductible, and policy limit 3 levels.</t>
+  </si>
+  <si>
+    <t>% Loss deductible with min and max deductible</t>
+  </si>
+  <si>
+    <t>% Loss deductible with min and max deductible 2nd level. Calcrule 19</t>
   </si>
 </sst>
 </file>
@@ -814,23 +817,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:K44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="101.5546875" customWidth="1"/>
-    <col min="8" max="9" width="22.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="101.5703125" customWidth="1"/>
+    <col min="8" max="9" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
         <v>43</v>
       </c>
@@ -841,7 +844,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
@@ -871,7 +874,7 @@
       </c>
       <c r="K4" s="3"/>
     </row>
-    <row r="5" spans="2:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>8</v>
       </c>
@@ -898,7 +901,7 @@
       </c>
       <c r="J5" s="5"/>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>4</v>
       </c>
@@ -925,7 +928,7 @@
       </c>
       <c r="J6" s="5"/>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>12</v>
       </c>
@@ -952,7 +955,7 @@
       </c>
       <c r="J7" s="7"/>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>46</v>
       </c>
@@ -960,7 +963,7 @@
         <v>47</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E8" s="7">
         <v>1</v>
@@ -979,7 +982,7 @@
       </c>
       <c r="J8" s="5"/>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>51</v>
       </c>
@@ -987,7 +990,7 @@
         <v>50</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E9" s="5">
         <v>1</v>
@@ -1006,7 +1009,7 @@
       </c>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>53</v>
       </c>
@@ -1014,7 +1017,7 @@
         <v>52</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E10" s="5">
         <v>1</v>
@@ -1033,7 +1036,7 @@
       </c>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>55</v>
       </c>
@@ -1041,7 +1044,7 @@
         <v>54</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E11" s="7">
         <v>1</v>
@@ -1060,7 +1063,7 @@
       </c>
       <c r="J11" s="5"/>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>57</v>
       </c>
@@ -1068,7 +1071,7 @@
         <v>56</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E12" s="7" t="s">
         <v>58</v>
@@ -1087,7 +1090,7 @@
       </c>
       <c r="J12" s="5"/>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>60</v>
       </c>
@@ -1095,7 +1098,7 @@
         <v>68</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E13" s="7">
         <v>10</v>
@@ -1114,7 +1117,7 @@
       </c>
       <c r="J13" s="7"/>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>62</v>
       </c>
@@ -1122,7 +1125,7 @@
         <v>69</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E14" s="7">
         <v>11</v>
@@ -1141,7 +1144,7 @@
       </c>
       <c r="J14" s="7"/>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>63</v>
       </c>
@@ -1149,7 +1152,7 @@
         <v>70</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E15" s="7">
         <v>3</v>
@@ -1168,7 +1171,7 @@
       </c>
       <c r="J15" s="7"/>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>64</v>
       </c>
@@ -1176,7 +1179,7 @@
         <v>65</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E16" s="7">
         <v>5</v>
@@ -1195,7 +1198,7 @@
       </c>
       <c r="J16" s="7"/>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>71</v>
       </c>
@@ -1203,7 +1206,7 @@
         <v>89</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E17" t="s">
         <v>83</v>
@@ -1222,7 +1225,7 @@
       </c>
       <c r="J17" s="7"/>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>72</v>
       </c>
@@ -1230,7 +1233,7 @@
         <v>73</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E18" s="8" t="s">
         <v>74</v>
@@ -1249,7 +1252,7 @@
       </c>
       <c r="J18" s="7"/>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>77</v>
       </c>
@@ -1257,7 +1260,7 @@
         <v>80</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E19" s="7">
         <v>16</v>
@@ -1276,7 +1279,7 @@
       </c>
       <c r="J19" s="7"/>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>78</v>
       </c>
@@ -1284,7 +1287,7 @@
         <v>79</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E20" s="7">
         <v>15</v>
@@ -1303,7 +1306,7 @@
       </c>
       <c r="J20" s="7"/>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>81</v>
       </c>
@@ -1311,7 +1314,7 @@
         <v>82</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E21" s="7">
         <v>9</v>
@@ -1330,20 +1333,34 @@
       </c>
       <c r="J21" s="7"/>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
+      <c r="C22" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="E22">
+        <v>19</v>
+      </c>
+      <c r="F22" s="7">
+        <v>1</v>
+      </c>
+      <c r="G22" s="7">
+        <v>1</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>61</v>
+      </c>
       <c r="J22" s="7"/>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>85</v>
       </c>
@@ -1356,7 +1373,7 @@
       <c r="I23" s="5"/>
       <c r="J23" s="7"/>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>86</v>
       </c>
@@ -1364,7 +1381,7 @@
         <v>107</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E24" s="7">
         <v>1</v>
@@ -1383,7 +1400,7 @@
       </c>
       <c r="J24" s="7"/>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>88</v>
       </c>
@@ -1394,15 +1411,15 @@
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>90</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E26" s="7">
         <v>10</v>
@@ -1420,7 +1437,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>91</v>
       </c>
@@ -1430,7 +1447,7 @@
       <c r="H27" s="5"/>
       <c r="I27" s="5"/>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>92</v>
       </c>
@@ -1456,7 +1473,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>94</v>
       </c>
@@ -1479,7 +1496,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>96</v>
       </c>
@@ -1505,7 +1522,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>97</v>
       </c>
@@ -1531,7 +1548,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>98</v>
       </c>
@@ -1557,7 +1574,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>99</v>
       </c>
@@ -1571,7 +1588,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>108</v>
       </c>
@@ -1597,7 +1614,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>109</v>
       </c>
@@ -1623,7 +1640,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>114</v>
       </c>
@@ -1649,7 +1666,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>117</v>
       </c>
@@ -1675,7 +1692,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B38" s="5" t="s">
         <v>119</v>
       </c>
@@ -1701,7 +1718,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B39" s="5" t="s">
         <v>120</v>
       </c>
@@ -1727,21 +1744,21 @@
         <v>61</v>
       </c>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B40" s="5" t="s">
         <v>123</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="D40" s="5">
-        <v>0</v>
+        <v>136</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>133</v>
       </c>
       <c r="E40">
         <v>19</v>
       </c>
       <c r="F40" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G40" s="7">
         <v>1</v>
@@ -1753,12 +1770,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B41" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C41" s="5" t="s">
         <v>125</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>126</v>
       </c>
       <c r="D41" s="5">
         <v>0</v>
@@ -1779,12 +1796,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B42" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C42" s="5" t="s">
         <v>127</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>128</v>
       </c>
       <c r="D42" s="5" t="s">
         <v>87</v>
@@ -1805,32 +1822,32 @@
         <v>61</v>
       </c>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B43" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C43" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="C43" s="5" t="s">
+      <c r="H43" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="I43" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B44" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="H43" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="I43" s="5" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B44" s="5" t="s">
+      <c r="C44" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="C44" s="5" t="s">
+      <c r="H44" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="H44" s="5" t="s">
-        <v>133</v>
-      </c>
       <c r="I44" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -1846,22 +1863,22 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="61.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.21875" customWidth="1"/>
-    <col min="5" max="5" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="G2" s="3" t="s">
         <v>33</v>
       </c>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>17</v>
       </c>
@@ -1881,7 +1898,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>21</v>
       </c>
@@ -1901,7 +1918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>22</v>
       </c>
@@ -1921,7 +1938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>23</v>
       </c>
@@ -1941,7 +1958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>24</v>
       </c>
@@ -1961,7 +1978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>25</v>
       </c>
@@ -1981,7 +1998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>26</v>
       </c>
@@ -2001,7 +2018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="9" t="s">
         <v>27</v>
       </c>
@@ -2021,7 +2038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="9" t="s">
         <v>28</v>
       </c>
@@ -2041,7 +2058,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="9" t="s">
         <v>29</v>
       </c>
@@ -2061,7 +2078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>30</v>
       </c>
@@ -2081,7 +2098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>31</v>
       </c>
@@ -2101,7 +2118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>32</v>
       </c>
@@ -2121,7 +2138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>75</v>
       </c>
@@ -2141,7 +2158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
         <v>76</v>
       </c>
@@ -2161,12 +2178,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="G18" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>40</v>
       </c>
@@ -2180,7 +2197,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
         <v>35</v>
       </c>
@@ -2194,7 +2211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
         <v>36</v>
       </c>
@@ -2208,7 +2225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
         <v>37</v>
       </c>
@@ -2222,7 +2239,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="9" t="s">
         <v>38</v>
       </c>
@@ -2236,7 +2253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="9" t="s">
         <v>39</v>
       </c>

</xml_diff>

<commit_message>
added test for new rule 21 - wip
</commit_message>
<xml_diff>
--- a/ftest/ftest.xlsx
+++ b/ftest/ftest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\Joh\git\ktest\ftest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28F2D4CB-7D72-4344-AB68-21AF083927A9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B5CADDB-E965-4132-9B16-FD68F1D31DC1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="11025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="138">
   <si>
     <t>yes</t>
   </si>
@@ -437,6 +437,9 @@
   </si>
   <si>
     <t>% Loss deductible with min and max deductible 2nd level. Calcrule 19</t>
+  </si>
+  <si>
+    <t>% TIV deductible with min and max deductible</t>
   </si>
 </sst>
 </file>
@@ -818,7 +821,7 @@
   <dimension ref="B1:K44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1364,13 +1367,27 @@
       <c r="B23" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="C23" s="5"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
+      <c r="C23" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="E23" s="7">
+        <v>21</v>
+      </c>
+      <c r="F23" s="7">
+        <v>1</v>
+      </c>
+      <c r="G23" s="7">
+        <v>1</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>132</v>
+      </c>
       <c r="J23" s="7"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
new tests for OED primary t&c
</commit_message>
<xml_diff>
--- a/ftest/ftest.xlsx
+++ b/ftest/ftest.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\Joh\git\ktest\ftest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B5CADDB-E965-4132-9B16-FD68F1D31DC1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52D4B09B-8581-4B1C-8B66-5E3DFC59BF2F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="11025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="11028" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ftests" sheetId="1" r:id="rId1"/>
     <sheet name="test parameters" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="142">
   <si>
     <t>yes</t>
   </si>
@@ -440,6 +440,18 @@
   </si>
   <si>
     <t>% TIV deductible with min and max deductible</t>
+  </si>
+  <si>
+    <t>fm40</t>
+  </si>
+  <si>
+    <t>OED spec example 5 - multiple policy layers</t>
+  </si>
+  <si>
+    <t>fm41</t>
+  </si>
+  <si>
+    <t>A single special condition on locations 1 and 2, based on OED spec example 3</t>
   </si>
 </sst>
 </file>
@@ -818,25 +830,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:K44"/>
+  <dimension ref="B1:K46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="101.5703125" customWidth="1"/>
-    <col min="8" max="9" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="101.5546875" customWidth="1"/>
+    <col min="8" max="9" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
       <c r="D3" t="s">
         <v>43</v>
       </c>
@@ -847,7 +859,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
@@ -877,7 +889,7 @@
       </c>
       <c r="K4" s="3"/>
     </row>
-    <row r="5" spans="2:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B5" s="5" t="s">
         <v>8</v>
       </c>
@@ -904,7 +916,7 @@
       </c>
       <c r="J5" s="5"/>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B6" s="5" t="s">
         <v>4</v>
       </c>
@@ -931,7 +943,7 @@
       </c>
       <c r="J6" s="5"/>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B7" s="5" t="s">
         <v>12</v>
       </c>
@@ -958,7 +970,7 @@
       </c>
       <c r="J7" s="7"/>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B8" s="5" t="s">
         <v>46</v>
       </c>
@@ -985,7 +997,7 @@
       </c>
       <c r="J8" s="5"/>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B9" s="5" t="s">
         <v>51</v>
       </c>
@@ -1012,7 +1024,7 @@
       </c>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B10" s="5" t="s">
         <v>53</v>
       </c>
@@ -1039,7 +1051,7 @@
       </c>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B11" s="5" t="s">
         <v>55</v>
       </c>
@@ -1066,7 +1078,7 @@
       </c>
       <c r="J11" s="5"/>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B12" s="5" t="s">
         <v>57</v>
       </c>
@@ -1093,7 +1105,7 @@
       </c>
       <c r="J12" s="5"/>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B13" s="5" t="s">
         <v>60</v>
       </c>
@@ -1120,7 +1132,7 @@
       </c>
       <c r="J13" s="7"/>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B14" s="5" t="s">
         <v>62</v>
       </c>
@@ -1147,7 +1159,7 @@
       </c>
       <c r="J14" s="7"/>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B15" s="5" t="s">
         <v>63</v>
       </c>
@@ -1174,7 +1186,7 @@
       </c>
       <c r="J15" s="7"/>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B16" s="5" t="s">
         <v>64</v>
       </c>
@@ -1201,7 +1213,7 @@
       </c>
       <c r="J16" s="7"/>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B17" s="5" t="s">
         <v>71</v>
       </c>
@@ -1228,7 +1240,7 @@
       </c>
       <c r="J17" s="7"/>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B18" s="5" t="s">
         <v>72</v>
       </c>
@@ -1255,7 +1267,7 @@
       </c>
       <c r="J18" s="7"/>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B19" s="5" t="s">
         <v>77</v>
       </c>
@@ -1282,7 +1294,7 @@
       </c>
       <c r="J19" s="7"/>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B20" s="5" t="s">
         <v>78</v>
       </c>
@@ -1309,7 +1321,7 @@
       </c>
       <c r="J20" s="7"/>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B21" s="5" t="s">
         <v>81</v>
       </c>
@@ -1336,7 +1348,7 @@
       </c>
       <c r="J21" s="7"/>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B22" s="5" t="s">
         <v>84</v>
       </c>
@@ -1363,7 +1375,7 @@
       </c>
       <c r="J22" s="7"/>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B23" s="5" t="s">
         <v>85</v>
       </c>
@@ -1390,7 +1402,7 @@
       </c>
       <c r="J23" s="7"/>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B24" s="5" t="s">
         <v>86</v>
       </c>
@@ -1417,7 +1429,7 @@
       </c>
       <c r="J24" s="7"/>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B25" s="5" t="s">
         <v>88</v>
       </c>
@@ -1428,7 +1440,7 @@
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B26" s="5" t="s">
         <v>90</v>
       </c>
@@ -1454,7 +1466,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B27" s="5" t="s">
         <v>91</v>
       </c>
@@ -1464,7 +1476,7 @@
       <c r="H27" s="5"/>
       <c r="I27" s="5"/>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B28" s="5" t="s">
         <v>92</v>
       </c>
@@ -1490,7 +1502,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B29" s="5" t="s">
         <v>94</v>
       </c>
@@ -1513,7 +1525,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B30" s="5" t="s">
         <v>96</v>
       </c>
@@ -1539,7 +1551,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B31" s="5" t="s">
         <v>97</v>
       </c>
@@ -1565,7 +1577,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B32" s="5" t="s">
         <v>98</v>
       </c>
@@ -1591,7 +1603,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B33" s="5" t="s">
         <v>99</v>
       </c>
@@ -1605,7 +1617,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B34" s="5" t="s">
         <v>108</v>
       </c>
@@ -1631,7 +1643,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B35" s="5" t="s">
         <v>109</v>
       </c>
@@ -1657,7 +1669,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B36" s="5" t="s">
         <v>114</v>
       </c>
@@ -1683,7 +1695,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B37" s="5" t="s">
         <v>117</v>
       </c>
@@ -1709,7 +1721,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B38" s="5" t="s">
         <v>119</v>
       </c>
@@ -1735,7 +1747,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B39" s="5" t="s">
         <v>120</v>
       </c>
@@ -1761,7 +1773,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B40" s="5" t="s">
         <v>123</v>
       </c>
@@ -1787,7 +1799,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B41" s="5" t="s">
         <v>124</v>
       </c>
@@ -1813,7 +1825,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B42" s="5" t="s">
         <v>126</v>
       </c>
@@ -1839,7 +1851,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B43" s="5" t="s">
         <v>128</v>
       </c>
@@ -1853,7 +1865,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B44" s="5" t="s">
         <v>130</v>
       </c>
@@ -1864,6 +1876,46 @@
         <v>132</v>
       </c>
       <c r="I44" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B45" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="D45" t="s">
+        <v>133</v>
+      </c>
+      <c r="G45" s="7">
+        <v>2</v>
+      </c>
+      <c r="H45" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="I45" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B46" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="D46" t="s">
+        <v>133</v>
+      </c>
+      <c r="G46" s="7">
+        <v>1</v>
+      </c>
+      <c r="H46" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="I46" s="5" t="s">
         <v>132</v>
       </c>
     </row>
@@ -1880,22 +1932,22 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="61.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
       <c r="G2" s="3" t="s">
         <v>33</v>
       </c>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>17</v>
       </c>
@@ -1915,7 +1967,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>21</v>
       </c>
@@ -1935,7 +1987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>22</v>
       </c>
@@ -1955,7 +2007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>23</v>
       </c>
@@ -1975,7 +2027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
         <v>24</v>
       </c>
@@ -1995,7 +2047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
         <v>25</v>
       </c>
@@ -2015,7 +2067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>26</v>
       </c>
@@ -2035,7 +2087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B10" s="9" t="s">
         <v>27</v>
       </c>
@@ -2055,7 +2107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B11" s="9" t="s">
         <v>28</v>
       </c>
@@ -2075,7 +2127,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B12" s="9" t="s">
         <v>29</v>
       </c>
@@ -2095,7 +2147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
         <v>30</v>
       </c>
@@ -2115,7 +2167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>31</v>
       </c>
@@ -2135,7 +2187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
         <v>32</v>
       </c>
@@ -2155,7 +2207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="s">
         <v>75</v>
       </c>
@@ -2175,7 +2227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
         <v>76</v>
       </c>
@@ -2195,12 +2247,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
       <c r="G18" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
         <v>40</v>
       </c>
@@ -2214,7 +2266,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B20" s="2" t="s">
         <v>35</v>
       </c>
@@ -2228,7 +2280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B21" s="2" t="s">
         <v>36</v>
       </c>
@@ -2242,7 +2294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B22" s="2" t="s">
         <v>37</v>
       </c>
@@ -2256,7 +2308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B23" s="9" t="s">
         <v>38</v>
       </c>
@@ -2270,7 +2322,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B24" s="9" t="s">
         <v>39</v>
       </c>

</xml_diff>

<commit_message>
added test case for investigation
</commit_message>
<xml_diff>
--- a/ftest/ftest.xlsx
+++ b/ftest/ftest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\Joh\git\ktest\ftest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\msys64_2\home\Joh\ktest\ftest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52D4B09B-8581-4B1C-8B66-5E3DFC59BF2F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB3FFF83-56E1-45A8-A50A-56001878916A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="11028" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ftests" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="145">
   <si>
     <t>yes</t>
   </si>
@@ -452,6 +452,15 @@
   </si>
   <si>
     <t>A single special condition on locations 1 and 2, based on OED spec example 3</t>
+  </si>
+  <si>
+    <t>fm42</t>
+  </si>
+  <si>
+    <t>12,14,24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test case for investigation of issue in net loss calculations for allocrule 1 and 0 </t>
   </si>
 </sst>
 </file>
@@ -830,25 +839,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:K46"/>
+  <dimension ref="B1:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="3" width="101.5546875" customWidth="1"/>
+    <col min="3" max="3" width="101.53125" customWidth="1"/>
     <col min="8" max="9" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.46484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.45">
       <c r="D3" t="s">
         <v>43</v>
       </c>
@@ -859,7 +868,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
@@ -889,7 +898,7 @@
       </c>
       <c r="K4" s="3"/>
     </row>
-    <row r="5" spans="2:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:11" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B5" s="5" t="s">
         <v>8</v>
       </c>
@@ -916,7 +925,7 @@
       </c>
       <c r="J5" s="5"/>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B6" s="5" t="s">
         <v>4</v>
       </c>
@@ -943,7 +952,7 @@
       </c>
       <c r="J6" s="5"/>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B7" s="5" t="s">
         <v>12</v>
       </c>
@@ -970,7 +979,7 @@
       </c>
       <c r="J7" s="7"/>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B8" s="5" t="s">
         <v>46</v>
       </c>
@@ -997,7 +1006,7 @@
       </c>
       <c r="J8" s="5"/>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B9" s="5" t="s">
         <v>51</v>
       </c>
@@ -1024,7 +1033,7 @@
       </c>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B10" s="5" t="s">
         <v>53</v>
       </c>
@@ -1051,7 +1060,7 @@
       </c>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B11" s="5" t="s">
         <v>55</v>
       </c>
@@ -1078,7 +1087,7 @@
       </c>
       <c r="J11" s="5"/>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B12" s="5" t="s">
         <v>57</v>
       </c>
@@ -1105,7 +1114,7 @@
       </c>
       <c r="J12" s="5"/>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B13" s="5" t="s">
         <v>60</v>
       </c>
@@ -1132,7 +1141,7 @@
       </c>
       <c r="J13" s="7"/>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B14" s="5" t="s">
         <v>62</v>
       </c>
@@ -1159,7 +1168,7 @@
       </c>
       <c r="J14" s="7"/>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B15" s="5" t="s">
         <v>63</v>
       </c>
@@ -1186,7 +1195,7 @@
       </c>
       <c r="J15" s="7"/>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B16" s="5" t="s">
         <v>64</v>
       </c>
@@ -1213,7 +1222,7 @@
       </c>
       <c r="J16" s="7"/>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B17" s="5" t="s">
         <v>71</v>
       </c>
@@ -1240,7 +1249,7 @@
       </c>
       <c r="J17" s="7"/>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B18" s="5" t="s">
         <v>72</v>
       </c>
@@ -1267,7 +1276,7 @@
       </c>
       <c r="J18" s="7"/>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B19" s="5" t="s">
         <v>77</v>
       </c>
@@ -1294,7 +1303,7 @@
       </c>
       <c r="J19" s="7"/>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B20" s="5" t="s">
         <v>78</v>
       </c>
@@ -1321,7 +1330,7 @@
       </c>
       <c r="J20" s="7"/>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B21" s="5" t="s">
         <v>81</v>
       </c>
@@ -1348,7 +1357,7 @@
       </c>
       <c r="J21" s="7"/>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B22" s="5" t="s">
         <v>84</v>
       </c>
@@ -1375,7 +1384,7 @@
       </c>
       <c r="J22" s="7"/>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B23" s="5" t="s">
         <v>85</v>
       </c>
@@ -1402,7 +1411,7 @@
       </c>
       <c r="J23" s="7"/>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B24" s="5" t="s">
         <v>86</v>
       </c>
@@ -1429,7 +1438,7 @@
       </c>
       <c r="J24" s="7"/>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B25" s="5" t="s">
         <v>88</v>
       </c>
@@ -1440,7 +1449,7 @@
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B26" s="5" t="s">
         <v>90</v>
       </c>
@@ -1466,7 +1475,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B27" s="5" t="s">
         <v>91</v>
       </c>
@@ -1476,7 +1485,7 @@
       <c r="H27" s="5"/>
       <c r="I27" s="5"/>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B28" s="5" t="s">
         <v>92</v>
       </c>
@@ -1502,7 +1511,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B29" s="5" t="s">
         <v>94</v>
       </c>
@@ -1525,7 +1534,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B30" s="5" t="s">
         <v>96</v>
       </c>
@@ -1551,7 +1560,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B31" s="5" t="s">
         <v>97</v>
       </c>
@@ -1577,7 +1586,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B32" s="5" t="s">
         <v>98</v>
       </c>
@@ -1603,7 +1612,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B33" s="5" t="s">
         <v>99</v>
       </c>
@@ -1617,7 +1626,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B34" s="5" t="s">
         <v>108</v>
       </c>
@@ -1643,7 +1652,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B35" s="5" t="s">
         <v>109</v>
       </c>
@@ -1669,7 +1678,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B36" s="5" t="s">
         <v>114</v>
       </c>
@@ -1695,7 +1704,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B37" s="5" t="s">
         <v>117</v>
       </c>
@@ -1721,7 +1730,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B38" s="5" t="s">
         <v>119</v>
       </c>
@@ -1747,7 +1756,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B39" s="5" t="s">
         <v>120</v>
       </c>
@@ -1773,7 +1782,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B40" s="5" t="s">
         <v>123</v>
       </c>
@@ -1799,7 +1808,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B41" s="5" t="s">
         <v>124</v>
       </c>
@@ -1825,7 +1834,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B42" s="5" t="s">
         <v>126</v>
       </c>
@@ -1851,7 +1860,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B43" s="5" t="s">
         <v>128</v>
       </c>
@@ -1865,7 +1874,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B44" s="5" t="s">
         <v>130</v>
       </c>
@@ -1879,7 +1888,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B45" s="5" t="s">
         <v>138</v>
       </c>
@@ -1899,7 +1908,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B46" s="5" t="s">
         <v>140</v>
       </c>
@@ -1916,6 +1925,32 @@
         <v>132</v>
       </c>
       <c r="I46" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="47" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B47" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="D47" t="s">
+        <v>133</v>
+      </c>
+      <c r="E47" t="s">
+        <v>143</v>
+      </c>
+      <c r="F47">
+        <v>2</v>
+      </c>
+      <c r="G47" s="7">
+        <v>1</v>
+      </c>
+      <c r="H47" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="I47" s="5" t="s">
         <v>132</v>
       </c>
     </row>
@@ -1932,7 +1967,7 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="61.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
@@ -1941,13 +1976,13 @@
     <col min="9" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.45">
       <c r="G2" s="3" t="s">
         <v>33</v>
       </c>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B3" s="1" t="s">
         <v>17</v>
       </c>
@@ -1967,7 +2002,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B4" s="2" t="s">
         <v>21</v>
       </c>
@@ -1987,7 +2022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B5" s="2" t="s">
         <v>22</v>
       </c>
@@ -2007,7 +2042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B6" s="2" t="s">
         <v>23</v>
       </c>
@@ -2027,7 +2062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B7" s="2" t="s">
         <v>24</v>
       </c>
@@ -2047,7 +2082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B8" s="2" t="s">
         <v>25</v>
       </c>
@@ -2067,7 +2102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B9" s="2" t="s">
         <v>26</v>
       </c>
@@ -2087,7 +2122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B10" s="9" t="s">
         <v>27</v>
       </c>
@@ -2107,7 +2142,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B11" s="9" t="s">
         <v>28</v>
       </c>
@@ -2127,7 +2162,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B12" s="9" t="s">
         <v>29</v>
       </c>
@@ -2147,7 +2182,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B13" s="2" t="s">
         <v>30</v>
       </c>
@@ -2167,7 +2202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B14" s="2" t="s">
         <v>31</v>
       </c>
@@ -2187,7 +2222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B15" s="2" t="s">
         <v>32</v>
       </c>
@@ -2207,7 +2242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B16" s="2" t="s">
         <v>75</v>
       </c>
@@ -2227,7 +2262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B17" s="2" t="s">
         <v>76</v>
       </c>
@@ -2247,12 +2282,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.45">
       <c r="G18" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B19" s="1" t="s">
         <v>40</v>
       </c>
@@ -2266,7 +2301,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B20" s="2" t="s">
         <v>35</v>
       </c>
@@ -2280,7 +2315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B21" s="2" t="s">
         <v>36</v>
       </c>
@@ -2294,7 +2329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B22" s="2" t="s">
         <v>37</v>
       </c>
@@ -2308,7 +2343,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B23" s="9" t="s">
         <v>38</v>
       </c>
@@ -2322,7 +2357,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B24" s="9" t="s">
         <v>39</v>
       </c>

</xml_diff>

<commit_message>
added test for allocrule2 fix
</commit_message>
<xml_diff>
--- a/ftest/ftest.xlsx
+++ b/ftest/ftest.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\msys64_2\home\Joh\ktest\ftest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\msys64\home\Joh\ktest\ftest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB3FFF83-56E1-45A8-A50A-56001878916A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DD0AF88-821F-4089-92EA-32E08C77552B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ftests" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="148">
   <si>
     <t>yes</t>
   </si>
@@ -461,6 +461,15 @@
   </si>
   <si>
     <t xml:space="preserve">Test case for investigation of issue in net loss calculations for allocrule 1 and 0 </t>
+  </si>
+  <si>
+    <t>fm43</t>
+  </si>
+  <si>
+    <t>Multiple accounts with different number of layers (policies) per account. Account level output</t>
+  </si>
+  <si>
+    <t>2,12,14</t>
   </si>
 </sst>
 </file>
@@ -541,10 +550,10 @@
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -557,7 +566,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -839,25 +848,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:K47"/>
+  <dimension ref="B1:K48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="101.53125" customWidth="1"/>
+    <col min="3" max="3" width="101.5546875" customWidth="1"/>
     <col min="8" max="9" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.46484375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
       <c r="D3" t="s">
         <v>43</v>
       </c>
@@ -868,7 +877,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
@@ -898,7 +907,7 @@
       </c>
       <c r="K4" s="3"/>
     </row>
-    <row r="5" spans="2:11" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B5" s="5" t="s">
         <v>8</v>
       </c>
@@ -925,7 +934,7 @@
       </c>
       <c r="J5" s="5"/>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B6" s="5" t="s">
         <v>4</v>
       </c>
@@ -952,7 +961,7 @@
       </c>
       <c r="J6" s="5"/>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B7" s="5" t="s">
         <v>12</v>
       </c>
@@ -979,7 +988,7 @@
       </c>
       <c r="J7" s="7"/>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B8" s="5" t="s">
         <v>46</v>
       </c>
@@ -1006,7 +1015,7 @@
       </c>
       <c r="J8" s="5"/>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B9" s="5" t="s">
         <v>51</v>
       </c>
@@ -1033,7 +1042,7 @@
       </c>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B10" s="5" t="s">
         <v>53</v>
       </c>
@@ -1060,7 +1069,7 @@
       </c>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B11" s="5" t="s">
         <v>55</v>
       </c>
@@ -1087,7 +1096,7 @@
       </c>
       <c r="J11" s="5"/>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B12" s="5" t="s">
         <v>57</v>
       </c>
@@ -1114,7 +1123,7 @@
       </c>
       <c r="J12" s="5"/>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B13" s="5" t="s">
         <v>60</v>
       </c>
@@ -1141,7 +1150,7 @@
       </c>
       <c r="J13" s="7"/>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B14" s="5" t="s">
         <v>62</v>
       </c>
@@ -1168,7 +1177,7 @@
       </c>
       <c r="J14" s="7"/>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B15" s="5" t="s">
         <v>63</v>
       </c>
@@ -1195,7 +1204,7 @@
       </c>
       <c r="J15" s="7"/>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B16" s="5" t="s">
         <v>64</v>
       </c>
@@ -1222,7 +1231,7 @@
       </c>
       <c r="J16" s="7"/>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B17" s="5" t="s">
         <v>71</v>
       </c>
@@ -1249,7 +1258,7 @@
       </c>
       <c r="J17" s="7"/>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B18" s="5" t="s">
         <v>72</v>
       </c>
@@ -1276,7 +1285,7 @@
       </c>
       <c r="J18" s="7"/>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B19" s="5" t="s">
         <v>77</v>
       </c>
@@ -1303,7 +1312,7 @@
       </c>
       <c r="J19" s="7"/>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B20" s="5" t="s">
         <v>78</v>
       </c>
@@ -1330,7 +1339,7 @@
       </c>
       <c r="J20" s="7"/>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B21" s="5" t="s">
         <v>81</v>
       </c>
@@ -1357,7 +1366,7 @@
       </c>
       <c r="J21" s="7"/>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B22" s="5" t="s">
         <v>84</v>
       </c>
@@ -1384,7 +1393,7 @@
       </c>
       <c r="J22" s="7"/>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B23" s="5" t="s">
         <v>85</v>
       </c>
@@ -1411,7 +1420,7 @@
       </c>
       <c r="J23" s="7"/>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B24" s="5" t="s">
         <v>86</v>
       </c>
@@ -1438,7 +1447,7 @@
       </c>
       <c r="J24" s="7"/>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B25" s="5" t="s">
         <v>88</v>
       </c>
@@ -1449,7 +1458,7 @@
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B26" s="5" t="s">
         <v>90</v>
       </c>
@@ -1475,7 +1484,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B27" s="5" t="s">
         <v>91</v>
       </c>
@@ -1485,7 +1494,7 @@
       <c r="H27" s="5"/>
       <c r="I27" s="5"/>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B28" s="5" t="s">
         <v>92</v>
       </c>
@@ -1511,7 +1520,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B29" s="5" t="s">
         <v>94</v>
       </c>
@@ -1534,7 +1543,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B30" s="5" t="s">
         <v>96</v>
       </c>
@@ -1560,7 +1569,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="31" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B31" s="5" t="s">
         <v>97</v>
       </c>
@@ -1586,7 +1595,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B32" s="5" t="s">
         <v>98</v>
       </c>
@@ -1612,7 +1621,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B33" s="5" t="s">
         <v>99</v>
       </c>
@@ -1626,7 +1635,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B34" s="5" t="s">
         <v>108</v>
       </c>
@@ -1652,7 +1661,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B35" s="5" t="s">
         <v>109</v>
       </c>
@@ -1678,7 +1687,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B36" s="5" t="s">
         <v>114</v>
       </c>
@@ -1704,7 +1713,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B37" s="5" t="s">
         <v>117</v>
       </c>
@@ -1730,7 +1739,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B38" s="5" t="s">
         <v>119</v>
       </c>
@@ -1756,7 +1765,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B39" s="5" t="s">
         <v>120</v>
       </c>
@@ -1782,7 +1791,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B40" s="5" t="s">
         <v>123</v>
       </c>
@@ -1808,7 +1817,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B41" s="5" t="s">
         <v>124</v>
       </c>
@@ -1834,7 +1843,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B42" s="5" t="s">
         <v>126</v>
       </c>
@@ -1860,7 +1869,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B43" s="5" t="s">
         <v>128</v>
       </c>
@@ -1874,7 +1883,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B44" s="5" t="s">
         <v>130</v>
       </c>
@@ -1888,7 +1897,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="45" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B45" s="5" t="s">
         <v>138</v>
       </c>
@@ -1908,7 +1917,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="46" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B46" s="5" t="s">
         <v>140</v>
       </c>
@@ -1928,7 +1937,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="47" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B47" s="5" t="s">
         <v>142</v>
       </c>
@@ -1951,6 +1960,32 @@
         <v>132</v>
       </c>
       <c r="I47" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="48" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B48" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="D48" t="s">
+        <v>133</v>
+      </c>
+      <c r="E48" t="s">
+        <v>147</v>
+      </c>
+      <c r="F48">
+        <v>3</v>
+      </c>
+      <c r="G48" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H48" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="I48" s="5" t="s">
         <v>132</v>
       </c>
     </row>
@@ -1967,7 +2002,7 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="61.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
@@ -1976,13 +2011,13 @@
     <col min="9" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
       <c r="G2" s="3" t="s">
         <v>33</v>
       </c>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>17</v>
       </c>
@@ -2002,7 +2037,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>21</v>
       </c>
@@ -2022,7 +2057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>22</v>
       </c>
@@ -2042,7 +2077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>23</v>
       </c>
@@ -2062,7 +2097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
         <v>24</v>
       </c>
@@ -2082,7 +2117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
         <v>25</v>
       </c>
@@ -2102,7 +2137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>26</v>
       </c>
@@ -2122,7 +2157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B10" s="9" t="s">
         <v>27</v>
       </c>
@@ -2142,7 +2177,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B11" s="9" t="s">
         <v>28</v>
       </c>
@@ -2162,7 +2197,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B12" s="9" t="s">
         <v>29</v>
       </c>
@@ -2182,7 +2217,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
         <v>30</v>
       </c>
@@ -2202,7 +2237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>31</v>
       </c>
@@ -2222,7 +2257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
         <v>32</v>
       </c>
@@ -2242,7 +2277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="s">
         <v>75</v>
       </c>
@@ -2262,7 +2297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
         <v>76</v>
       </c>
@@ -2282,12 +2317,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
       <c r="G18" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
         <v>40</v>
       </c>
@@ -2301,7 +2336,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B20" s="2" t="s">
         <v>35</v>
       </c>
@@ -2315,7 +2350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B21" s="2" t="s">
         <v>36</v>
       </c>
@@ -2329,7 +2364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B22" s="2" t="s">
         <v>37</v>
       </c>
@@ -2343,7 +2378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B23" s="9" t="s">
         <v>38</v>
       </c>
@@ -2357,7 +2392,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B24" s="9" t="s">
         <v>39</v>
       </c>

</xml_diff>

<commit_message>
added test for symmetric layers fm44
</commit_message>
<xml_diff>
--- a/ftest/ftest.xlsx
+++ b/ftest/ftest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\msys64\home\Joh\ktest\ftest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DD0AF88-821F-4089-92EA-32E08C77552B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9F1560D-57AE-48F5-A143-2F2647A31B79}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="150">
   <si>
     <t>yes</t>
   </si>
@@ -470,6 +470,12 @@
   </si>
   <si>
     <t>2,12,14</t>
+  </si>
+  <si>
+    <t>Multiple accounts with same number of layers (policies) per account. Account level output</t>
+  </si>
+  <si>
+    <t>fm44</t>
   </si>
 </sst>
 </file>
@@ -848,10 +854,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:K48"/>
+  <dimension ref="B1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1957,10 +1963,10 @@
         <v>1</v>
       </c>
       <c r="H47" s="5" t="s">
-        <v>132</v>
+        <v>61</v>
       </c>
       <c r="I47" s="5" t="s">
-        <v>132</v>
+        <v>61</v>
       </c>
     </row>
     <row r="48" spans="2:9" x14ac:dyDescent="0.3">
@@ -1987,6 +1993,32 @@
       </c>
       <c r="I48" s="5" t="s">
         <v>132</v>
+      </c>
+    </row>
+    <row r="49" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B49" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="D49" t="s">
+        <v>133</v>
+      </c>
+      <c r="E49" t="s">
+        <v>147</v>
+      </c>
+      <c r="F49">
+        <v>3</v>
+      </c>
+      <c r="G49" s="7">
+        <v>2</v>
+      </c>
+      <c r="H49" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="I49" s="5" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added tests for min and max deductible under over limit scenario
</commit_message>
<xml_diff>
--- a/ftest/ftest.xlsx
+++ b/ftest/ftest.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\msys64\home\Joh\ktest\ftest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CBE28B7-D8BB-425C-A44C-D87239685A1F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A31B8526-073E-4913-BD69-05CCF8E915F3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="384" windowWidth="23040" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="158">
   <si>
     <t>yes</t>
   </si>
@@ -479,6 +479,27 @@
   </si>
   <si>
     <t>Test case to investigate sidx -3 issues</t>
+  </si>
+  <si>
+    <t>fm45</t>
+  </si>
+  <si>
+    <t>Min deductible under-limit scenario</t>
+  </si>
+  <si>
+    <t>1, 8</t>
+  </si>
+  <si>
+    <t>fm47</t>
+  </si>
+  <si>
+    <t>fm48</t>
+  </si>
+  <si>
+    <t>Max deductible over-limit scenario</t>
+  </si>
+  <si>
+    <t>1,7</t>
   </si>
 </sst>
 </file>
@@ -857,10 +878,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:K50"/>
+  <dimension ref="B1:K52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="G50" sqref="G50"/>
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1900,10 +1921,10 @@
         <v>131</v>
       </c>
       <c r="H44" s="5" t="s">
-        <v>132</v>
+        <v>61</v>
       </c>
       <c r="I44" s="5" t="s">
-        <v>132</v>
+        <v>61</v>
       </c>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.3">
@@ -1920,10 +1941,10 @@
         <v>2</v>
       </c>
       <c r="H45" s="5" t="s">
-        <v>132</v>
+        <v>61</v>
       </c>
       <c r="I45" s="5" t="s">
-        <v>132</v>
+        <v>61</v>
       </c>
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.3">
@@ -1940,10 +1961,10 @@
         <v>1</v>
       </c>
       <c r="H46" s="5" t="s">
-        <v>132</v>
+        <v>61</v>
       </c>
       <c r="I46" s="5" t="s">
-        <v>132</v>
+        <v>61</v>
       </c>
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.3">
@@ -2026,7 +2047,7 @@
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B50" s="5" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>150</v>
@@ -2044,10 +2065,62 @@
         <v>41</v>
       </c>
       <c r="H50" s="5" t="s">
-        <v>132</v>
+        <v>61</v>
       </c>
       <c r="I50" s="5" t="s">
-        <v>132</v>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B51" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="D51" t="s">
+        <v>133</v>
+      </c>
+      <c r="E51" t="s">
+        <v>153</v>
+      </c>
+      <c r="F51">
+        <v>2</v>
+      </c>
+      <c r="G51" s="7">
+        <v>1</v>
+      </c>
+      <c r="H51" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="I51" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="52" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B52" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="D52" t="s">
+        <v>133</v>
+      </c>
+      <c r="E52" t="s">
+        <v>157</v>
+      </c>
+      <c r="F52">
+        <v>2</v>
+      </c>
+      <c r="G52" s="7">
+        <v>1</v>
+      </c>
+      <c r="H52" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="I52" s="5" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test case for nested sublimits
</commit_message>
<xml_diff>
--- a/ftest/ftest.xlsx
+++ b/ftest/ftest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\msys64\home\Joh\ktest\ftest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\msys64_2\home\Joh\ktest_new\ftest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A31B8526-073E-4913-BD69-05CCF8E915F3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{269A1800-9C4E-4B5D-9ED8-DF39C1895D85}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="384" windowWidth="23040" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ftests" sheetId="1" r:id="rId1"/>
@@ -21,12 +21,17 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="163">
   <si>
     <t>yes</t>
   </si>
@@ -500,6 +505,21 @@
   </si>
   <si>
     <t>1,7</t>
+  </si>
+  <si>
+    <t>Min Max deductible over-under limit scenario</t>
+  </si>
+  <si>
+    <t>1,12,10,8</t>
+  </si>
+  <si>
+    <t>fm49</t>
+  </si>
+  <si>
+    <t>fm50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OED spec example 4 - nested sublimits </t>
   </si>
 </sst>
 </file>
@@ -878,10 +898,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:K52"/>
+  <dimension ref="B1:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="I54" sqref="I54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2121,6 +2141,49 @@
       </c>
       <c r="I52" s="5" t="s">
         <v>61</v>
+      </c>
+    </row>
+    <row r="53" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B53" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="D53" t="s">
+        <v>133</v>
+      </c>
+      <c r="E53" t="s">
+        <v>159</v>
+      </c>
+      <c r="F53">
+        <v>3</v>
+      </c>
+      <c r="G53" s="7">
+        <v>1</v>
+      </c>
+      <c r="H53" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="I53" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="54" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B54" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="D54" t="s">
+        <v>133</v>
+      </c>
+      <c r="H54" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="I54" s="5" t="s">
+        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added test for calcrule 26
</commit_message>
<xml_diff>
--- a/ftest/ftest.xlsx
+++ b/ftest/ftest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\msys64_2\home\Joh\ktest_new\ftest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{269A1800-9C4E-4B5D-9ED8-DF39C1895D85}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACB03B14-C425-467E-90D8-3DE86FFEB801}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="3444" windowWidth="17280" windowHeight="8916" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ftests" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="164">
   <si>
     <t>yes</t>
   </si>
@@ -520,6 +520,9 @@
   </si>
   <si>
     <t xml:space="preserve">OED spec example 4 - nested sublimits </t>
+  </si>
+  <si>
+    <t>% TIV deductible with min and max deductible (converting % TIV deductible to an amount)</t>
   </si>
 </sst>
 </file>
@@ -900,8 +903,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="I54" sqref="I54"/>
+    <sheetView tabSelected="1" topLeftCell="D16" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1501,12 +1504,27 @@
       <c r="B25" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
+      <c r="C25" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="E25" s="7">
+        <v>26</v>
+      </c>
+      <c r="F25" s="7">
+        <v>1</v>
+      </c>
+      <c r="G25" s="7">
+        <v>1</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B26" s="5" t="s">

</xml_diff>

<commit_message>
test cases for debug #54 and #55
</commit_message>
<xml_diff>
--- a/ftest/ftest.xlsx
+++ b/ftest/ftest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\msys64_2\home\Joh\ktest_new\ftest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACB03B14-C425-467E-90D8-3DE86FFEB801}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5301A198-7F75-4089-AEE7-7204C74EDA45}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="3444" windowWidth="17280" windowHeight="8916" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ftests" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="168">
   <si>
     <t>yes</t>
   </si>
@@ -523,6 +523,18 @@
   </si>
   <si>
     <t>% TIV deductible with min and max deductible (converting % TIV deductible to an amount)</t>
+  </si>
+  <si>
+    <t>fm51</t>
+  </si>
+  <si>
+    <t>fm52</t>
+  </si>
+  <si>
+    <t>Zero intermediate loss example (max deductible) #54</t>
+  </si>
+  <si>
+    <t>Max deductible not being applied for some samples #55</t>
   </si>
 </sst>
 </file>
@@ -901,25 +913,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:K54"/>
+  <dimension ref="B1:K56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D16" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="H56" sqref="H56:I56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="101.5546875" customWidth="1"/>
-    <col min="8" max="9" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="101.5703125" customWidth="1"/>
+    <col min="8" max="9" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
         <v>43</v>
       </c>
@@ -930,7 +942,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
@@ -960,7 +972,7 @@
       </c>
       <c r="K4" s="3"/>
     </row>
-    <row r="5" spans="2:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>8</v>
       </c>
@@ -987,7 +999,7 @@
       </c>
       <c r="J5" s="5"/>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>4</v>
       </c>
@@ -1014,7 +1026,7 @@
       </c>
       <c r="J6" s="5"/>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>12</v>
       </c>
@@ -1041,7 +1053,7 @@
       </c>
       <c r="J7" s="7"/>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>46</v>
       </c>
@@ -1068,7 +1080,7 @@
       </c>
       <c r="J8" s="5"/>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>51</v>
       </c>
@@ -1095,7 +1107,7 @@
       </c>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>53</v>
       </c>
@@ -1122,7 +1134,7 @@
       </c>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>55</v>
       </c>
@@ -1149,7 +1161,7 @@
       </c>
       <c r="J11" s="5"/>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>57</v>
       </c>
@@ -1176,7 +1188,7 @@
       </c>
       <c r="J12" s="5"/>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>60</v>
       </c>
@@ -1203,7 +1215,7 @@
       </c>
       <c r="J13" s="7"/>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>62</v>
       </c>
@@ -1230,7 +1242,7 @@
       </c>
       <c r="J14" s="7"/>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>63</v>
       </c>
@@ -1257,7 +1269,7 @@
       </c>
       <c r="J15" s="7"/>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>64</v>
       </c>
@@ -1284,7 +1296,7 @@
       </c>
       <c r="J16" s="7"/>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>71</v>
       </c>
@@ -1311,7 +1323,7 @@
       </c>
       <c r="J17" s="7"/>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>72</v>
       </c>
@@ -1338,7 +1350,7 @@
       </c>
       <c r="J18" s="7"/>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>77</v>
       </c>
@@ -1365,7 +1377,7 @@
       </c>
       <c r="J19" s="7"/>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>78</v>
       </c>
@@ -1392,7 +1404,7 @@
       </c>
       <c r="J20" s="7"/>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>81</v>
       </c>
@@ -1419,7 +1431,7 @@
       </c>
       <c r="J21" s="7"/>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>84</v>
       </c>
@@ -1446,7 +1458,7 @@
       </c>
       <c r="J22" s="7"/>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>85</v>
       </c>
@@ -1473,7 +1485,7 @@
       </c>
       <c r="J23" s="7"/>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>86</v>
       </c>
@@ -1500,7 +1512,7 @@
       </c>
       <c r="J24" s="7"/>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>88</v>
       </c>
@@ -1526,7 +1538,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>90</v>
       </c>
@@ -1552,7 +1564,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>91</v>
       </c>
@@ -1562,7 +1574,7 @@
       <c r="H27" s="5"/>
       <c r="I27" s="5"/>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>92</v>
       </c>
@@ -1588,7 +1600,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>94</v>
       </c>
@@ -1611,7 +1623,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>96</v>
       </c>
@@ -1637,7 +1649,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>97</v>
       </c>
@@ -1663,7 +1675,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>98</v>
       </c>
@@ -1689,7 +1701,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>99</v>
       </c>
@@ -1703,7 +1715,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>108</v>
       </c>
@@ -1729,7 +1741,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>109</v>
       </c>
@@ -1755,7 +1767,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>114</v>
       </c>
@@ -1781,7 +1793,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>117</v>
       </c>
@@ -1807,7 +1819,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B38" s="5" t="s">
         <v>119</v>
       </c>
@@ -1833,7 +1845,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B39" s="5" t="s">
         <v>120</v>
       </c>
@@ -1859,7 +1871,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B40" s="5" t="s">
         <v>123</v>
       </c>
@@ -1885,7 +1897,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B41" s="5" t="s">
         <v>124</v>
       </c>
@@ -1911,7 +1923,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B42" s="5" t="s">
         <v>126</v>
       </c>
@@ -1937,7 +1949,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B43" s="5" t="s">
         <v>128</v>
       </c>
@@ -1951,7 +1963,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B44" s="5" t="s">
         <v>130</v>
       </c>
@@ -1965,7 +1977,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B45" s="5" t="s">
         <v>138</v>
       </c>
@@ -1985,7 +1997,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B46" s="5" t="s">
         <v>140</v>
       </c>
@@ -2005,7 +2017,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B47" s="5" t="s">
         <v>142</v>
       </c>
@@ -2031,7 +2043,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B48" s="5" t="s">
         <v>145</v>
       </c>
@@ -2057,7 +2069,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B49" s="5" t="s">
         <v>149</v>
       </c>
@@ -2083,7 +2095,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B50" s="5" t="s">
         <v>151</v>
       </c>
@@ -2109,7 +2121,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B51" s="5" t="s">
         <v>154</v>
       </c>
@@ -2135,7 +2147,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B52" s="5" t="s">
         <v>155</v>
       </c>
@@ -2161,7 +2173,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B53" s="5" t="s">
         <v>160</v>
       </c>
@@ -2187,7 +2199,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B54" s="5" t="s">
         <v>161</v>
       </c>
@@ -2201,6 +2213,37 @@
         <v>132</v>
       </c>
       <c r="I54" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B55" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="D55" t="s">
+        <v>133</v>
+      </c>
+      <c r="H55" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="I55" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B56" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="H56" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="I56" s="5" t="s">
         <v>132</v>
       </c>
     </row>
@@ -2217,22 +2260,22 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="61.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="G2" s="3" t="s">
         <v>33</v>
       </c>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>17</v>
       </c>
@@ -2252,7 +2295,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>21</v>
       </c>
@@ -2272,7 +2315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>22</v>
       </c>
@@ -2292,7 +2335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>23</v>
       </c>
@@ -2312,7 +2355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>24</v>
       </c>
@@ -2332,7 +2375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>25</v>
       </c>
@@ -2352,7 +2395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>26</v>
       </c>
@@ -2372,7 +2415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="9" t="s">
         <v>27</v>
       </c>
@@ -2392,7 +2435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="9" t="s">
         <v>28</v>
       </c>
@@ -2412,7 +2455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="9" t="s">
         <v>29</v>
       </c>
@@ -2432,7 +2475,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>30</v>
       </c>
@@ -2452,7 +2495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>31</v>
       </c>
@@ -2472,7 +2515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>32</v>
       </c>
@@ -2492,7 +2535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>75</v>
       </c>
@@ -2512,7 +2555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
         <v>76</v>
       </c>
@@ -2532,12 +2575,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="G18" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>40</v>
       </c>
@@ -2551,7 +2594,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
         <v>35</v>
       </c>
@@ -2565,7 +2608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
         <v>36</v>
       </c>
@@ -2579,7 +2622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
         <v>37</v>
       </c>
@@ -2593,7 +2636,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="9" t="s">
         <v>38</v>
       </c>
@@ -2607,7 +2650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="9" t="s">
         <v>39</v>
       </c>

</xml_diff>

<commit_message>
finished test case for ktools issue #54
</commit_message>
<xml_diff>
--- a/ftest/ftest.xlsx
+++ b/ftest/ftest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\msys64_2\home\Joh\ktest_new\ftest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\msys64\home\Joh\ktest_new\ftest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5301A198-7F75-4089-AEE7-7204C74EDA45}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C575DC36-BBA0-4F79-AE29-49C189761032}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ftests" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="168">
   <si>
     <t>yes</t>
   </si>
@@ -534,7 +534,7 @@
     <t>Zero intermediate loss example (max deductible) #54</t>
   </si>
   <si>
-    <t>Max deductible not being applied for some samples #55</t>
+    <t>Max deductible not being applied for some samples #55. Need to fix over-limit logic</t>
   </si>
 </sst>
 </file>
@@ -915,23 +915,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:K56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="H56" sqref="H56:I56"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="101.5703125" customWidth="1"/>
-    <col min="8" max="9" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="101.5546875" customWidth="1"/>
+    <col min="8" max="9" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
       <c r="D3" t="s">
         <v>43</v>
       </c>
@@ -942,7 +942,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
@@ -972,7 +972,7 @@
       </c>
       <c r="K4" s="3"/>
     </row>
-    <row r="5" spans="2:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B5" s="5" t="s">
         <v>8</v>
       </c>
@@ -999,7 +999,7 @@
       </c>
       <c r="J5" s="5"/>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B6" s="5" t="s">
         <v>4</v>
       </c>
@@ -1026,7 +1026,7 @@
       </c>
       <c r="J6" s="5"/>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B7" s="5" t="s">
         <v>12</v>
       </c>
@@ -1053,7 +1053,7 @@
       </c>
       <c r="J7" s="7"/>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B8" s="5" t="s">
         <v>46</v>
       </c>
@@ -1080,7 +1080,7 @@
       </c>
       <c r="J8" s="5"/>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B9" s="5" t="s">
         <v>51</v>
       </c>
@@ -1107,7 +1107,7 @@
       </c>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B10" s="5" t="s">
         <v>53</v>
       </c>
@@ -1134,7 +1134,7 @@
       </c>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B11" s="5" t="s">
         <v>55</v>
       </c>
@@ -1161,7 +1161,7 @@
       </c>
       <c r="J11" s="5"/>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B12" s="5" t="s">
         <v>57</v>
       </c>
@@ -1188,7 +1188,7 @@
       </c>
       <c r="J12" s="5"/>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B13" s="5" t="s">
         <v>60</v>
       </c>
@@ -1215,7 +1215,7 @@
       </c>
       <c r="J13" s="7"/>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B14" s="5" t="s">
         <v>62</v>
       </c>
@@ -1242,7 +1242,7 @@
       </c>
       <c r="J14" s="7"/>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B15" s="5" t="s">
         <v>63</v>
       </c>
@@ -1269,7 +1269,7 @@
       </c>
       <c r="J15" s="7"/>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B16" s="5" t="s">
         <v>64</v>
       </c>
@@ -1296,7 +1296,7 @@
       </c>
       <c r="J16" s="7"/>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B17" s="5" t="s">
         <v>71</v>
       </c>
@@ -1323,7 +1323,7 @@
       </c>
       <c r="J17" s="7"/>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B18" s="5" t="s">
         <v>72</v>
       </c>
@@ -1350,7 +1350,7 @@
       </c>
       <c r="J18" s="7"/>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B19" s="5" t="s">
         <v>77</v>
       </c>
@@ -1377,7 +1377,7 @@
       </c>
       <c r="J19" s="7"/>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B20" s="5" t="s">
         <v>78</v>
       </c>
@@ -1404,7 +1404,7 @@
       </c>
       <c r="J20" s="7"/>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B21" s="5" t="s">
         <v>81</v>
       </c>
@@ -1431,7 +1431,7 @@
       </c>
       <c r="J21" s="7"/>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B22" s="5" t="s">
         <v>84</v>
       </c>
@@ -1458,7 +1458,7 @@
       </c>
       <c r="J22" s="7"/>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B23" s="5" t="s">
         <v>85</v>
       </c>
@@ -1485,7 +1485,7 @@
       </c>
       <c r="J23" s="7"/>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B24" s="5" t="s">
         <v>86</v>
       </c>
@@ -1512,7 +1512,7 @@
       </c>
       <c r="J24" s="7"/>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B25" s="5" t="s">
         <v>88</v>
       </c>
@@ -1538,7 +1538,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B26" s="5" t="s">
         <v>90</v>
       </c>
@@ -1564,7 +1564,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B27" s="5" t="s">
         <v>91</v>
       </c>
@@ -1574,7 +1574,7 @@
       <c r="H27" s="5"/>
       <c r="I27" s="5"/>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B28" s="5" t="s">
         <v>92</v>
       </c>
@@ -1600,7 +1600,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B29" s="5" t="s">
         <v>94</v>
       </c>
@@ -1623,7 +1623,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B30" s="5" t="s">
         <v>96</v>
       </c>
@@ -1649,7 +1649,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B31" s="5" t="s">
         <v>97</v>
       </c>
@@ -1675,7 +1675,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B32" s="5" t="s">
         <v>98</v>
       </c>
@@ -1701,7 +1701,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B33" s="5" t="s">
         <v>99</v>
       </c>
@@ -1715,7 +1715,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B34" s="5" t="s">
         <v>108</v>
       </c>
@@ -1741,7 +1741,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B35" s="5" t="s">
         <v>109</v>
       </c>
@@ -1767,7 +1767,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B36" s="5" t="s">
         <v>114</v>
       </c>
@@ -1793,7 +1793,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B37" s="5" t="s">
         <v>117</v>
       </c>
@@ -1819,7 +1819,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B38" s="5" t="s">
         <v>119</v>
       </c>
@@ -1845,7 +1845,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B39" s="5" t="s">
         <v>120</v>
       </c>
@@ -1871,7 +1871,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B40" s="5" t="s">
         <v>123</v>
       </c>
@@ -1897,7 +1897,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B41" s="5" t="s">
         <v>124</v>
       </c>
@@ -1923,7 +1923,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B42" s="5" t="s">
         <v>126</v>
       </c>
@@ -1949,7 +1949,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B43" s="5" t="s">
         <v>128</v>
       </c>
@@ -1963,7 +1963,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B44" s="5" t="s">
         <v>130</v>
       </c>
@@ -1977,7 +1977,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B45" s="5" t="s">
         <v>138</v>
       </c>
@@ -1997,7 +1997,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B46" s="5" t="s">
         <v>140</v>
       </c>
@@ -2017,7 +2017,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B47" s="5" t="s">
         <v>142</v>
       </c>
@@ -2043,7 +2043,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B48" s="5" t="s">
         <v>145</v>
       </c>
@@ -2069,7 +2069,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B49" s="5" t="s">
         <v>149</v>
       </c>
@@ -2095,7 +2095,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B50" s="5" t="s">
         <v>151</v>
       </c>
@@ -2121,7 +2121,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B51" s="5" t="s">
         <v>154</v>
       </c>
@@ -2147,7 +2147,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B52" s="5" t="s">
         <v>155</v>
       </c>
@@ -2173,7 +2173,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B53" s="5" t="s">
         <v>160</v>
       </c>
@@ -2199,7 +2199,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B54" s="5" t="s">
         <v>161</v>
       </c>
@@ -2216,7 +2216,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B55" s="5" t="s">
         <v>164</v>
       </c>
@@ -2227,18 +2227,21 @@
         <v>133</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>132</v>
+        <v>61</v>
       </c>
       <c r="I55" s="5" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="56" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B56" s="5" t="s">
         <v>165</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>167</v>
+      </c>
+      <c r="D56" t="s">
+        <v>133</v>
       </c>
       <c r="H56" s="5" t="s">
         <v>132</v>
@@ -2260,22 +2263,22 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="61.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
       <c r="G2" s="3" t="s">
         <v>33</v>
       </c>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>17</v>
       </c>
@@ -2295,7 +2298,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>21</v>
       </c>
@@ -2315,7 +2318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>22</v>
       </c>
@@ -2335,7 +2338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>23</v>
       </c>
@@ -2355,7 +2358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
         <v>24</v>
       </c>
@@ -2375,7 +2378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
         <v>25</v>
       </c>
@@ -2395,7 +2398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>26</v>
       </c>
@@ -2415,7 +2418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B10" s="9" t="s">
         <v>27</v>
       </c>
@@ -2435,7 +2438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B11" s="9" t="s">
         <v>28</v>
       </c>
@@ -2455,7 +2458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B12" s="9" t="s">
         <v>29</v>
       </c>
@@ -2475,7 +2478,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
         <v>30</v>
       </c>
@@ -2495,7 +2498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>31</v>
       </c>
@@ -2515,7 +2518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
         <v>32</v>
       </c>
@@ -2535,7 +2538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="s">
         <v>75</v>
       </c>
@@ -2555,7 +2558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
         <v>76</v>
       </c>
@@ -2575,12 +2578,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
       <c r="G18" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
         <v>40</v>
       </c>
@@ -2594,7 +2597,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B20" s="2" t="s">
         <v>35</v>
       </c>
@@ -2608,7 +2611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B21" s="2" t="s">
         <v>36</v>
       </c>
@@ -2622,7 +2625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B22" s="2" t="s">
         <v>37</v>
       </c>
@@ -2636,7 +2639,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B23" s="9" t="s">
         <v>38</v>
       </c>
@@ -2650,7 +2653,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B24" s="9" t="s">
         <v>39</v>
       </c>

</xml_diff>

<commit_message>
added test case fm53 for step policies
</commit_message>
<xml_diff>
--- a/ftest/ftest.xlsx
+++ b/ftest/ftest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\msys64\home\Joh\ktest_new\ftest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\msys64_2\home\Joh\ktest_new4\ftest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C575DC36-BBA0-4F79-AE29-49C189761032}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87D77AEE-5D8E-40F8-8D55-6EA1186E8165}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ftests" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="170">
   <si>
     <t>yes</t>
   </si>
@@ -535,6 +535,12 @@
   </si>
   <si>
     <t>Max deductible not being applied for some samples #55. Need to fix over-limit logic</t>
+  </si>
+  <si>
+    <t>fm53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JP Flood step policies with extra expense and debris removal </t>
   </si>
 </sst>
 </file>
@@ -913,25 +919,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:K56"/>
+  <dimension ref="B1:K57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="H56" sqref="H56:I56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="101.5546875" customWidth="1"/>
-    <col min="8" max="9" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="101.5703125" customWidth="1"/>
+    <col min="8" max="9" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
         <v>43</v>
       </c>
@@ -942,7 +948,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
@@ -972,7 +978,7 @@
       </c>
       <c r="K4" s="3"/>
     </row>
-    <row r="5" spans="2:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>8</v>
       </c>
@@ -999,7 +1005,7 @@
       </c>
       <c r="J5" s="5"/>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>4</v>
       </c>
@@ -1026,7 +1032,7 @@
       </c>
       <c r="J6" s="5"/>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>12</v>
       </c>
@@ -1053,7 +1059,7 @@
       </c>
       <c r="J7" s="7"/>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>46</v>
       </c>
@@ -1080,7 +1086,7 @@
       </c>
       <c r="J8" s="5"/>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>51</v>
       </c>
@@ -1107,7 +1113,7 @@
       </c>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>53</v>
       </c>
@@ -1134,7 +1140,7 @@
       </c>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>55</v>
       </c>
@@ -1161,7 +1167,7 @@
       </c>
       <c r="J11" s="5"/>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>57</v>
       </c>
@@ -1188,7 +1194,7 @@
       </c>
       <c r="J12" s="5"/>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>60</v>
       </c>
@@ -1215,7 +1221,7 @@
       </c>
       <c r="J13" s="7"/>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>62</v>
       </c>
@@ -1242,7 +1248,7 @@
       </c>
       <c r="J14" s="7"/>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>63</v>
       </c>
@@ -1269,7 +1275,7 @@
       </c>
       <c r="J15" s="7"/>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>64</v>
       </c>
@@ -1296,7 +1302,7 @@
       </c>
       <c r="J16" s="7"/>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>71</v>
       </c>
@@ -1323,7 +1329,7 @@
       </c>
       <c r="J17" s="7"/>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>72</v>
       </c>
@@ -1350,7 +1356,7 @@
       </c>
       <c r="J18" s="7"/>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>77</v>
       </c>
@@ -1377,7 +1383,7 @@
       </c>
       <c r="J19" s="7"/>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>78</v>
       </c>
@@ -1404,7 +1410,7 @@
       </c>
       <c r="J20" s="7"/>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>81</v>
       </c>
@@ -1431,7 +1437,7 @@
       </c>
       <c r="J21" s="7"/>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>84</v>
       </c>
@@ -1458,7 +1464,7 @@
       </c>
       <c r="J22" s="7"/>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>85</v>
       </c>
@@ -1485,7 +1491,7 @@
       </c>
       <c r="J23" s="7"/>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>86</v>
       </c>
@@ -1512,7 +1518,7 @@
       </c>
       <c r="J24" s="7"/>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>88</v>
       </c>
@@ -1538,7 +1544,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>90</v>
       </c>
@@ -1564,7 +1570,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>91</v>
       </c>
@@ -1574,7 +1580,7 @@
       <c r="H27" s="5"/>
       <c r="I27" s="5"/>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>92</v>
       </c>
@@ -1600,7 +1606,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>94</v>
       </c>
@@ -1623,7 +1629,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>96</v>
       </c>
@@ -1649,7 +1655,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>97</v>
       </c>
@@ -1675,7 +1681,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>98</v>
       </c>
@@ -1701,7 +1707,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>99</v>
       </c>
@@ -1715,7 +1721,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>108</v>
       </c>
@@ -1741,7 +1747,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>109</v>
       </c>
@@ -1767,7 +1773,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>114</v>
       </c>
@@ -1793,7 +1799,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>117</v>
       </c>
@@ -1819,7 +1825,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B38" s="5" t="s">
         <v>119</v>
       </c>
@@ -1845,7 +1851,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B39" s="5" t="s">
         <v>120</v>
       </c>
@@ -1871,7 +1877,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B40" s="5" t="s">
         <v>123</v>
       </c>
@@ -1897,7 +1903,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B41" s="5" t="s">
         <v>124</v>
       </c>
@@ -1923,7 +1929,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B42" s="5" t="s">
         <v>126</v>
       </c>
@@ -1949,7 +1955,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B43" s="5" t="s">
         <v>128</v>
       </c>
@@ -1957,13 +1963,13 @@
         <v>129</v>
       </c>
       <c r="H43" s="5" t="s">
-        <v>132</v>
+        <v>61</v>
       </c>
       <c r="I43" s="5" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B44" s="5" t="s">
         <v>130</v>
       </c>
@@ -1977,7 +1983,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B45" s="5" t="s">
         <v>138</v>
       </c>
@@ -1997,7 +2003,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B46" s="5" t="s">
         <v>140</v>
       </c>
@@ -2017,7 +2023,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B47" s="5" t="s">
         <v>142</v>
       </c>
@@ -2043,7 +2049,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B48" s="5" t="s">
         <v>145</v>
       </c>
@@ -2069,7 +2075,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B49" s="5" t="s">
         <v>149</v>
       </c>
@@ -2095,7 +2101,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B50" s="5" t="s">
         <v>151</v>
       </c>
@@ -2121,7 +2127,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B51" s="5" t="s">
         <v>154</v>
       </c>
@@ -2147,7 +2153,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B52" s="5" t="s">
         <v>155</v>
       </c>
@@ -2173,7 +2179,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B53" s="5" t="s">
         <v>160</v>
       </c>
@@ -2199,7 +2205,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B54" s="5" t="s">
         <v>161</v>
       </c>
@@ -2216,7 +2222,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B55" s="5" t="s">
         <v>164</v>
       </c>
@@ -2233,7 +2239,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B56" s="5" t="s">
         <v>165</v>
       </c>
@@ -2247,6 +2253,32 @@
         <v>132</v>
       </c>
       <c r="I56" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B57" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+      <c r="E57">
+        <v>27</v>
+      </c>
+      <c r="F57">
+        <v>1</v>
+      </c>
+      <c r="G57">
+        <v>1</v>
+      </c>
+      <c r="H57" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="I57" s="5" t="s">
         <v>132</v>
       </c>
     </row>
@@ -2263,22 +2295,22 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="61.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="G2" s="3" t="s">
         <v>33</v>
       </c>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>17</v>
       </c>
@@ -2298,7 +2330,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>21</v>
       </c>
@@ -2318,7 +2350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>22</v>
       </c>
@@ -2338,7 +2370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>23</v>
       </c>
@@ -2358,7 +2390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>24</v>
       </c>
@@ -2378,7 +2410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>25</v>
       </c>
@@ -2398,7 +2430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>26</v>
       </c>
@@ -2418,7 +2450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="9" t="s">
         <v>27</v>
       </c>
@@ -2438,7 +2470,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="9" t="s">
         <v>28</v>
       </c>
@@ -2458,7 +2490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="9" t="s">
         <v>29</v>
       </c>
@@ -2478,7 +2510,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>30</v>
       </c>
@@ -2498,7 +2530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>31</v>
       </c>
@@ -2518,7 +2550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>32</v>
       </c>
@@ -2538,7 +2570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>75</v>
       </c>
@@ -2558,7 +2590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
         <v>76</v>
       </c>
@@ -2578,12 +2610,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="G18" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>40</v>
       </c>
@@ -2597,7 +2629,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
         <v>35</v>
       </c>
@@ -2611,7 +2643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
         <v>36</v>
       </c>
@@ -2625,7 +2657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
         <v>37</v>
       </c>
@@ -2639,7 +2671,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="9" t="s">
         <v>38</v>
       </c>
@@ -2653,7 +2685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="9" t="s">
         <v>39</v>
       </c>

</xml_diff>

<commit_message>
completed test case to fix ktools #55
</commit_message>
<xml_diff>
--- a/ftest/ftest.xlsx
+++ b/ftest/ftest.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\msys64_2\home\Joh\ktest_new4\ftest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87D77AEE-5D8E-40F8-8D55-6EA1186E8165}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52C717EA-9D3D-463F-AF5D-A4654BEBB1F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="ftests" sheetId="1" r:id="rId1"/>
     <sheet name="test parameters" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="181029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -534,13 +534,13 @@
     <t>Zero intermediate loss example (max deductible) #54</t>
   </si>
   <si>
-    <t>Max deductible not being applied for some samples #55. Need to fix over-limit logic</t>
-  </si>
-  <si>
     <t>fm53</t>
   </si>
   <si>
     <t xml:space="preserve">JP Flood step policies with extra expense and debris removal </t>
+  </si>
+  <si>
+    <t>Max deductible not being applied for some samples #55.</t>
   </si>
 </sst>
 </file>
@@ -922,7 +922,7 @@
   <dimension ref="B1:K57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="H56" sqref="H56:I56"/>
+      <selection activeCell="I54" sqref="B54:I54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2244,24 +2244,24 @@
         <v>165</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="D56" t="s">
         <v>133</v>
       </c>
       <c r="H56" s="5" t="s">
-        <v>132</v>
+        <v>61</v>
       </c>
       <c r="I56" s="5" t="s">
-        <v>132</v>
+        <v>61</v>
       </c>
     </row>
     <row r="57" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B57" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="C57" s="5" t="s">
         <v>168</v>
-      </c>
-      <c r="C57" s="5" t="s">
-        <v>169</v>
       </c>
       <c r="D57">
         <v>0</v>

</xml_diff>

<commit_message>
added fm53 as regression test for ktools issue #54
</commit_message>
<xml_diff>
--- a/ftest/ftest.xlsx
+++ b/ftest/ftest.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\msys64_2\home\Joh\ktest_new4\ftest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52C717EA-9D3D-463F-AF5D-A4654BEBB1F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90CCC091-82AE-4C0F-ACB4-EBF1248C686C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="ftests" sheetId="1" r:id="rId1"/>
     <sheet name="test parameters" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029" iterateDelta="1E-4"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,6 +24,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="171">
   <si>
     <t>yes</t>
   </si>
@@ -537,10 +538,13 @@
     <t>fm53</t>
   </si>
   <si>
-    <t xml:space="preserve">JP Flood step policies with extra expense and debris removal </t>
-  </si>
-  <si>
     <t>Max deductible not being applied for some samples #55.</t>
+  </si>
+  <si>
+    <t>1,2,8,10,11,12,14</t>
+  </si>
+  <si>
+    <t>Max deductible not being applied for zero prior level losses (two levels back) #54</t>
   </si>
 </sst>
 </file>
@@ -921,8 +925,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:K57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="I54" sqref="B54:I54"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="H57" sqref="H57:I57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2244,7 +2248,7 @@
         <v>165</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D56" t="s">
         <v>133</v>
@@ -2261,25 +2265,25 @@
         <v>167</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="D57">
-        <v>0</v>
-      </c>
-      <c r="E57">
-        <v>27</v>
+        <v>2</v>
+      </c>
+      <c r="E57" t="s">
+        <v>169</v>
       </c>
       <c r="F57">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G57">
         <v>1</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>132</v>
+        <v>61</v>
       </c>
       <c r="I57" s="5" t="s">
-        <v>132</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test case for step policy
</commit_message>
<xml_diff>
--- a/ftest/ftest.xlsx
+++ b/ftest/ftest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\msys64_2\home\Joh\ktest_new4\ftest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90CCC091-82AE-4C0F-ACB4-EBF1248C686C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34B14325-DEB2-48AD-8D22-3349198B9E62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ftests" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="174">
   <si>
     <t>yes</t>
   </si>
@@ -545,6 +545,15 @@
   </si>
   <si>
     <t>Max deductible not being applied for zero prior level losses (two levels back) #54</t>
+  </si>
+  <si>
+    <t>fm54</t>
+  </si>
+  <si>
+    <t>JP Flood 3 step policy</t>
+  </si>
+  <si>
+    <t>27,28</t>
   </si>
 </sst>
 </file>
@@ -923,25 +932,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:K57"/>
+  <dimension ref="B1:K59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="H57" sqref="H57:I57"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="101.5703125" customWidth="1"/>
-    <col min="8" max="9" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="101.5546875" customWidth="1"/>
+    <col min="8" max="9" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
       <c r="D3" t="s">
         <v>43</v>
       </c>
@@ -952,7 +961,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
@@ -982,7 +991,7 @@
       </c>
       <c r="K4" s="3"/>
     </row>
-    <row r="5" spans="2:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B5" s="5" t="s">
         <v>8</v>
       </c>
@@ -1009,7 +1018,7 @@
       </c>
       <c r="J5" s="5"/>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B6" s="5" t="s">
         <v>4</v>
       </c>
@@ -1036,7 +1045,7 @@
       </c>
       <c r="J6" s="5"/>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B7" s="5" t="s">
         <v>12</v>
       </c>
@@ -1063,7 +1072,7 @@
       </c>
       <c r="J7" s="7"/>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B8" s="5" t="s">
         <v>46</v>
       </c>
@@ -1090,7 +1099,7 @@
       </c>
       <c r="J8" s="5"/>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B9" s="5" t="s">
         <v>51</v>
       </c>
@@ -1117,7 +1126,7 @@
       </c>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B10" s="5" t="s">
         <v>53</v>
       </c>
@@ -1144,7 +1153,7 @@
       </c>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B11" s="5" t="s">
         <v>55</v>
       </c>
@@ -1171,7 +1180,7 @@
       </c>
       <c r="J11" s="5"/>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B12" s="5" t="s">
         <v>57</v>
       </c>
@@ -1198,7 +1207,7 @@
       </c>
       <c r="J12" s="5"/>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B13" s="5" t="s">
         <v>60</v>
       </c>
@@ -1225,7 +1234,7 @@
       </c>
       <c r="J13" s="7"/>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B14" s="5" t="s">
         <v>62</v>
       </c>
@@ -1252,7 +1261,7 @@
       </c>
       <c r="J14" s="7"/>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B15" s="5" t="s">
         <v>63</v>
       </c>
@@ -1279,7 +1288,7 @@
       </c>
       <c r="J15" s="7"/>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B16" s="5" t="s">
         <v>64</v>
       </c>
@@ -1306,7 +1315,7 @@
       </c>
       <c r="J16" s="7"/>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B17" s="5" t="s">
         <v>71</v>
       </c>
@@ -1333,7 +1342,7 @@
       </c>
       <c r="J17" s="7"/>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B18" s="5" t="s">
         <v>72</v>
       </c>
@@ -1360,7 +1369,7 @@
       </c>
       <c r="J18" s="7"/>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B19" s="5" t="s">
         <v>77</v>
       </c>
@@ -1387,7 +1396,7 @@
       </c>
       <c r="J19" s="7"/>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B20" s="5" t="s">
         <v>78</v>
       </c>
@@ -1414,7 +1423,7 @@
       </c>
       <c r="J20" s="7"/>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B21" s="5" t="s">
         <v>81</v>
       </c>
@@ -1441,7 +1450,7 @@
       </c>
       <c r="J21" s="7"/>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B22" s="5" t="s">
         <v>84</v>
       </c>
@@ -1468,7 +1477,7 @@
       </c>
       <c r="J22" s="7"/>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B23" s="5" t="s">
         <v>85</v>
       </c>
@@ -1495,7 +1504,7 @@
       </c>
       <c r="J23" s="7"/>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B24" s="5" t="s">
         <v>86</v>
       </c>
@@ -1522,7 +1531,7 @@
       </c>
       <c r="J24" s="7"/>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B25" s="5" t="s">
         <v>88</v>
       </c>
@@ -1548,7 +1557,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B26" s="5" t="s">
         <v>90</v>
       </c>
@@ -1574,7 +1583,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B27" s="5" t="s">
         <v>91</v>
       </c>
@@ -1584,7 +1593,7 @@
       <c r="H27" s="5"/>
       <c r="I27" s="5"/>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B28" s="5" t="s">
         <v>92</v>
       </c>
@@ -1610,7 +1619,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B29" s="5" t="s">
         <v>94</v>
       </c>
@@ -1633,7 +1642,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B30" s="5" t="s">
         <v>96</v>
       </c>
@@ -1659,7 +1668,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B31" s="5" t="s">
         <v>97</v>
       </c>
@@ -1685,7 +1694,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B32" s="5" t="s">
         <v>98</v>
       </c>
@@ -1711,7 +1720,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B33" s="5" t="s">
         <v>99</v>
       </c>
@@ -1725,7 +1734,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B34" s="5" t="s">
         <v>108</v>
       </c>
@@ -1751,7 +1760,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B35" s="5" t="s">
         <v>109</v>
       </c>
@@ -1777,7 +1786,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B36" s="5" t="s">
         <v>114</v>
       </c>
@@ -1803,7 +1812,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B37" s="5" t="s">
         <v>117</v>
       </c>
@@ -1829,7 +1838,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B38" s="5" t="s">
         <v>119</v>
       </c>
@@ -1855,7 +1864,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B39" s="5" t="s">
         <v>120</v>
       </c>
@@ -1881,7 +1890,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B40" s="5" t="s">
         <v>123</v>
       </c>
@@ -1907,7 +1916,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B41" s="5" t="s">
         <v>124</v>
       </c>
@@ -1933,7 +1942,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B42" s="5" t="s">
         <v>126</v>
       </c>
@@ -1959,7 +1968,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B43" s="5" t="s">
         <v>128</v>
       </c>
@@ -1973,7 +1982,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B44" s="5" t="s">
         <v>130</v>
       </c>
@@ -1987,7 +1996,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B45" s="5" t="s">
         <v>138</v>
       </c>
@@ -2007,7 +2016,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B46" s="5" t="s">
         <v>140</v>
       </c>
@@ -2027,7 +2036,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B47" s="5" t="s">
         <v>142</v>
       </c>
@@ -2053,7 +2062,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B48" s="5" t="s">
         <v>145</v>
       </c>
@@ -2079,7 +2088,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B49" s="5" t="s">
         <v>149</v>
       </c>
@@ -2105,7 +2114,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B50" s="5" t="s">
         <v>151</v>
       </c>
@@ -2131,7 +2140,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B51" s="5" t="s">
         <v>154</v>
       </c>
@@ -2157,7 +2166,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B52" s="5" t="s">
         <v>155</v>
       </c>
@@ -2183,7 +2192,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B53" s="5" t="s">
         <v>160</v>
       </c>
@@ -2209,7 +2218,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B54" s="5" t="s">
         <v>161</v>
       </c>
@@ -2226,7 +2235,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B55" s="5" t="s">
         <v>164</v>
       </c>
@@ -2243,7 +2252,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B56" s="5" t="s">
         <v>165</v>
       </c>
@@ -2260,7 +2269,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B57" s="5" t="s">
         <v>167</v>
       </c>
@@ -2285,6 +2294,36 @@
       <c r="I57" s="5" t="s">
         <v>61</v>
       </c>
+    </row>
+    <row r="58" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B58" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="E58" t="s">
+        <v>173</v>
+      </c>
+      <c r="F58">
+        <v>1</v>
+      </c>
+      <c r="G58">
+        <v>1</v>
+      </c>
+      <c r="H58" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="I58" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="59" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="H59" s="5"/>
+      <c r="I59" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2299,22 +2338,22 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="61.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
       <c r="G2" s="3" t="s">
         <v>33</v>
       </c>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>17</v>
       </c>
@@ -2334,7 +2373,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>21</v>
       </c>
@@ -2354,7 +2393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>22</v>
       </c>
@@ -2374,7 +2413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>23</v>
       </c>
@@ -2394,7 +2433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
         <v>24</v>
       </c>
@@ -2414,7 +2453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
         <v>25</v>
       </c>
@@ -2434,7 +2473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>26</v>
       </c>
@@ -2454,7 +2493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B10" s="9" t="s">
         <v>27</v>
       </c>
@@ -2474,7 +2513,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B11" s="9" t="s">
         <v>28</v>
       </c>
@@ -2494,7 +2533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B12" s="9" t="s">
         <v>29</v>
       </c>
@@ -2514,7 +2553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
         <v>30</v>
       </c>
@@ -2534,7 +2573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>31</v>
       </c>
@@ -2554,7 +2593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
         <v>32</v>
       </c>
@@ -2574,7 +2613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="s">
         <v>75</v>
       </c>
@@ -2594,7 +2633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
         <v>76</v>
       </c>
@@ -2614,12 +2653,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
       <c r="G18" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
         <v>40</v>
       </c>
@@ -2633,7 +2672,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B20" s="2" t="s">
         <v>35</v>
       </c>
@@ -2647,7 +2686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B21" s="2" t="s">
         <v>36</v>
       </c>
@@ -2661,7 +2700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B22" s="2" t="s">
         <v>37</v>
       </c>
@@ -2675,7 +2714,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B23" s="9" t="s">
         <v>38</v>
       </c>
@@ -2689,7 +2728,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B24" s="9" t="s">
         <v>39</v>
       </c>

</xml_diff>

<commit_message>
added tests for jp flood general policies
</commit_message>
<xml_diff>
--- a/ftest/ftest.xlsx
+++ b/ftest/ftest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\msys64_2\home\Joh\ktest_new4\ftest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B485AD52-6B47-4BD3-A967-AC9E4ABA9833}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06036780-276A-461B-BC64-BC03FBBA8C62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ftests" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="181">
   <si>
     <t>yes</t>
   </si>
@@ -559,10 +559,22 @@
     <t>fm55</t>
   </si>
   <si>
-    <t>JP Flood all step policies unit test</t>
-  </si>
-  <si>
     <t>27,28,29,14</t>
+  </si>
+  <si>
+    <t>fm56</t>
+  </si>
+  <si>
+    <t>fm57</t>
+  </si>
+  <si>
+    <t>JP Flood general policy 'A2' with deductible</t>
+  </si>
+  <si>
+    <t>JP Flood all general policies unit test (T1 only)</t>
+  </si>
+  <si>
+    <t>JP Flood all step policies unit test (T1,2,3,5)</t>
   </si>
 </sst>
 </file>
@@ -941,10 +953,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:K59"/>
+  <dimension ref="B1:K61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="H59" sqref="H59:I59"/>
+    <sheetView tabSelected="1" topLeftCell="D43" workbookViewId="0">
+      <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2335,24 +2347,76 @@
         <v>174</v>
       </c>
       <c r="C59" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="D59">
+        <v>0</v>
+      </c>
+      <c r="E59" t="s">
         <v>175</v>
       </c>
-      <c r="D59">
-        <v>0</v>
-      </c>
-      <c r="E59" t="s">
+      <c r="F59">
+        <v>1</v>
+      </c>
+      <c r="G59">
+        <v>1</v>
+      </c>
+      <c r="H59" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="I59" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B60" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="F59">
-        <v>1</v>
-      </c>
-      <c r="G59">
-        <v>1</v>
-      </c>
-      <c r="H59" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="I59" s="5" t="s">
+      <c r="C60" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="D60">
+        <v>0</v>
+      </c>
+      <c r="E60">
+        <v>28</v>
+      </c>
+      <c r="F60">
+        <v>1</v>
+      </c>
+      <c r="G60">
+        <v>1</v>
+      </c>
+      <c r="H60" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="I60" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B61" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
+      <c r="E61">
+        <v>28</v>
+      </c>
+      <c r="F61">
+        <v>1</v>
+      </c>
+      <c r="G61">
+        <v>1</v>
+      </c>
+      <c r="H61" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="I61" s="5" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added test for various general step policies and calcrules 30 and 31
</commit_message>
<xml_diff>
--- a/ftest/ftest.xlsx
+++ b/ftest/ftest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\msys64_2\home\Joh\ktest_new4\ftest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06036780-276A-461B-BC64-BC03FBBA8C62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9CCBAF4-76BD-472D-A906-D09E4B745705}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ftests" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="184">
   <si>
     <t>yes</t>
   </si>
@@ -575,6 +575,15 @@
   </si>
   <si>
     <t>JP Flood all step policies unit test (T1,2,3,5)</t>
+  </si>
+  <si>
+    <t>fm58</t>
+  </si>
+  <si>
+    <t>Various generic step policies (T1,2,3,5)</t>
+  </si>
+  <si>
+    <t>27,28,30,31</t>
   </si>
 </sst>
 </file>
@@ -953,10 +962,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:K61"/>
+  <dimension ref="B1:K62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D43" workbookViewId="0">
-      <selection activeCell="D61" sqref="D61"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2417,6 +2426,32 @@
         <v>61</v>
       </c>
       <c r="I61" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B62" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="D62">
+        <v>0</v>
+      </c>
+      <c r="E62" t="s">
+        <v>183</v>
+      </c>
+      <c r="F62">
+        <v>1</v>
+      </c>
+      <c r="G62">
+        <v>1</v>
+      </c>
+      <c r="H62" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="I62" s="5" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added test for calcrule 32 stepped
</commit_message>
<xml_diff>
--- a/ftest/ftest.xlsx
+++ b/ftest/ftest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\msys64_2\home\Joh\ktest_new4\ftest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9CCBAF4-76BD-472D-A906-D09E4B745705}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DF3AA56-3449-4E0B-91B6-BB49AAFF626D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1905" yWindow="1905" windowWidth="11400" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ftests" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="187">
   <si>
     <t>yes</t>
   </si>
@@ -584,6 +584,15 @@
   </si>
   <si>
     <t>27,28,30,31</t>
+  </si>
+  <si>
+    <t>JP Flood Franchise policies unit test (T1,2,3,5)</t>
+  </si>
+  <si>
+    <t>fm59</t>
+  </si>
+  <si>
+    <t>28,32</t>
   </si>
 </sst>
 </file>
@@ -962,10 +971,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:K62"/>
+  <dimension ref="B1:K63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+      <selection activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2452,6 +2461,32 @@
         <v>61</v>
       </c>
       <c r="I62" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B63" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="D63">
+        <v>0</v>
+      </c>
+      <c r="E63" t="s">
+        <v>186</v>
+      </c>
+      <c r="F63">
+        <v>1</v>
+      </c>
+      <c r="G63">
+        <v>1</v>
+      </c>
+      <c r="H63" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="I63" s="5" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>